<commit_message>
Responsabilidades para zona común y administrador en conjuntos residenciales enriquesido
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/Event Storming/ConjuntosResidenciales - Event Storming.xlsx
+++ b/Doo-Doc/Nueva Version Victus/Event Storming/ConjuntosResidenciales - Event Storming.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Music\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228CA7C3-1FEA-4F81-A5A2-C4C4AB1FC31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6E5A14-D0A0-4C9B-9844-340D68CAD301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="3285" windowWidth="16800" windowHeight="14190" activeTab="2" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="2" activeTab="4" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
   </bookViews>
   <sheets>
     <sheet name="Flujo de eventos en el tiempo" sheetId="61" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="196">
   <si>
     <t>Descripción</t>
   </si>
@@ -530,9 +530,6 @@
     <t>Asegurar que el numero de contacto  del conjunto residencial que se desea registrar  no ha haya sido asignado previamente a otro conjunto residencial.</t>
   </si>
   <si>
-    <t>ConRes-Pol0008</t>
-  </si>
-  <si>
     <t>Registrar zona común</t>
   </si>
   <si>
@@ -630,6 +627,12 @@
   </si>
   <si>
     <t>Conjunto residencial modificador</t>
+  </si>
+  <si>
+    <t>ConRes-Pol0004</t>
+  </si>
+  <si>
+    <t>ConRes-Pol0005</t>
   </si>
 </sst>
 </file>
@@ -1263,86 +1266,191 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1351,111 +1459,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2020,8 +2023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{235BA608-57CC-45B0-8234-10CA49C3B004}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:C21"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2048,83 +2051,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="69"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="57"/>
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="53" t="str">
+      <c r="B3" s="64" t="str">
         <f>'Listado Objetos de Dominio'!B4</f>
         <v>Objeto de dominio que representa cada una de las comunidades habitacionales organizadas en un sistema. Abarca la totalidad de los elementos que componen el conjunto, desde las unidades habitacionales individuales (inmuebles) hasta las zonas comunes.</v>
       </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="54"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="65"/>
       <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="55"/>
+      <c r="C4" s="48"/>
       <c r="D4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="56"/>
-      <c r="G4" s="63" t="s">
+      <c r="F4" s="66"/>
+      <c r="G4" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="63"/>
+      <c r="H4" s="51"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -2134,52 +2137,52 @@
       <c r="K4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="66" t="s">
+      <c r="L4" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="67" t="s">
+      <c r="M4" s="55" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="57" t="s">
+      <c r="D5" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="56" t="s">
+      <c r="E5" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="56"/>
-      <c r="G5" s="61" t="s">
+      <c r="F5" s="66"/>
+      <c r="G5" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="61"/>
-      <c r="I5" s="64" t="s">
+      <c r="H5" s="49"/>
+      <c r="I5" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="65" t="s">
+      <c r="J5" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="62" t="s">
+      <c r="K5" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="66"/>
-      <c r="M5" s="67"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="55"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="60"/>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="58"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="68"/>
       <c r="E6" s="11" t="s">
         <v>21</v>
       </c>
@@ -2192,39 +2195,39 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="64"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="62"/>
-      <c r="L6" s="66"/>
-      <c r="M6" s="67"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="55"/>
     </row>
     <row r="7" spans="1:14" ht="87.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="47" t="s">
+      <c r="D7" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="44" t="s">
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="44" t="s">
+      <c r="H7" s="43" t="s">
         <v>158</v>
       </c>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47" t="s">
+      <c r="I7" s="58"/>
+      <c r="J7" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="K7" s="47"/>
-      <c r="L7" s="47" t="s">
+      <c r="K7" s="58"/>
+      <c r="L7" s="58" t="s">
         <v>36</v>
       </c>
       <c r="M7" s="26" t="s">
@@ -2232,104 +2235,104 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="51"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="48"/>
+      <c r="A8" s="62"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="59"/>
+      <c r="L8" s="59"/>
       <c r="M8" s="26" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="51"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
+      <c r="A9" s="62"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="59"/>
       <c r="M9" s="26" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="51"/>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="43" t="s">
+      <c r="A10" s="62"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="H10" s="43" t="s">
+      <c r="H10" s="69" t="s">
         <v>160</v>
       </c>
-      <c r="I10" s="48"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="48"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="59"/>
       <c r="M10" s="26" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="52"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="49"/>
-      <c r="K11" s="49"/>
-      <c r="L11" s="49"/>
+      <c r="A11" s="63"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="69"/>
+      <c r="H11" s="69"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="60"/>
       <c r="M11" s="26" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="50" t="s">
+      <c r="A12" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="47" t="s">
+      <c r="C12" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="47" t="s">
+      <c r="D12" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="44" t="s">
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="H12" s="44" t="s">
+      <c r="H12" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="I12" s="47"/>
-      <c r="J12" s="47" t="s">
+      <c r="I12" s="58"/>
+      <c r="J12" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="K12" s="47"/>
-      <c r="L12" s="47" t="s">
+      <c r="K12" s="58"/>
+      <c r="L12" s="58" t="s">
         <v>44</v>
       </c>
       <c r="M12" s="26" t="s">
@@ -2337,52 +2340,52 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="51"/>
-      <c r="B13" s="48"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="48"/>
+      <c r="A13" s="62"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="59"/>
+      <c r="K13" s="59"/>
+      <c r="L13" s="59"/>
       <c r="M13" s="26" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="51"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="48"/>
+      <c r="A14" s="62"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="59"/>
+      <c r="K14" s="59"/>
+      <c r="L14" s="59"/>
       <c r="M14" s="26" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="52"/>
-      <c r="B15" s="49"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="49"/>
-      <c r="L15" s="49"/>
+      <c r="A15" s="63"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="60"/>
+      <c r="L15" s="60"/>
       <c r="M15" s="26" t="s">
         <v>89</v>
       </c>
@@ -2392,21 +2395,21 @@
         <v>45</v>
       </c>
       <c r="B16" s="35" t="s">
+        <v>191</v>
+      </c>
+      <c r="C16" s="35" t="s">
         <v>192</v>
-      </c>
-      <c r="C16" s="35" t="s">
-        <v>193</v>
       </c>
       <c r="D16" s="35" t="s">
         <v>29</v>
       </c>
       <c r="E16" s="35"/>
       <c r="F16" s="35"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
       <c r="I16" s="35"/>
       <c r="J16" s="35" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K16" s="35"/>
       <c r="L16" s="35" t="s">
@@ -2431,10 +2434,10 @@
       </c>
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
-      <c r="G17" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="H17" s="43" t="s">
+      <c r="G17" s="69" t="s">
+        <v>194</v>
+      </c>
+      <c r="H17" s="69" t="s">
         <v>160</v>
       </c>
       <c r="I17" s="22"/>
@@ -2464,8 +2467,8 @@
       </c>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="69"/>
       <c r="I18" s="22"/>
       <c r="J18" s="22" t="s">
         <v>34</v>
@@ -2493,10 +2496,10 @@
       </c>
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
-      <c r="G19" s="44" t="s">
-        <v>161</v>
-      </c>
-      <c r="H19" s="44" t="s">
+      <c r="G19" s="43" t="s">
+        <v>195</v>
+      </c>
+      <c r="H19" s="43" t="s">
         <v>159</v>
       </c>
       <c r="I19" s="22"/>
@@ -2526,8 +2529,8 @@
       </c>
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
       <c r="I20" s="22"/>
       <c r="J20" s="22" t="s">
         <v>41</v>
@@ -2545,7 +2548,7 @@
         <v>45</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C21" s="22" t="s">
         <v>61</v>
@@ -2555,8 +2558,8 @@
       </c>
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="46"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="45"/>
       <c r="I21" s="22"/>
       <c r="J21" s="22" t="s">
         <v>36</v>
@@ -2571,6 +2574,37 @@
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="G12:G16"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="G19:G21"/>
+    <mergeCell ref="H19:H21"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="L12:L15"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="I12:I15"/>
+    <mergeCell ref="H12:H16"/>
+    <mergeCell ref="L7:L11"/>
+    <mergeCell ref="K7:K11"/>
+    <mergeCell ref="J7:J11"/>
+    <mergeCell ref="I7:I11"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="C7:C11"/>
     <mergeCell ref="G7:G9"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A5:A6"/>
@@ -2587,37 +2621,6 @@
     <mergeCell ref="B7:B11"/>
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="F7:F11"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="L7:L11"/>
-    <mergeCell ref="K7:K11"/>
-    <mergeCell ref="J7:J11"/>
-    <mergeCell ref="I7:I11"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="L12:L15"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="I12:I15"/>
-    <mergeCell ref="H12:H16"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="F12:F15"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="G12:G16"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="G19:G21"/>
-    <mergeCell ref="H19:H21"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
@@ -2636,7 +2639,7 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J20" sqref="J20"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2664,83 +2667,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="80"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="74"/>
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="81" t="str">
+      <c r="B3" s="75" t="str">
         <f>'Listado Objetos de Dominio'!$B$5</f>
         <v>Objeto de dominio que representa a cada una de las zonas comunes que se encuentran dentro de un conjunto residencial para que los residentes puedan reservar esos espacios y porder usarlos.</v>
       </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="83"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="77"/>
       <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="85"/>
+      <c r="C4" s="79"/>
       <c r="D4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="86" t="s">
+      <c r="E4" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="87"/>
-      <c r="G4" s="88" t="s">
+      <c r="F4" s="81"/>
+      <c r="G4" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="89"/>
+      <c r="H4" s="83"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -2750,52 +2753,52 @@
       <c r="K4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="90" t="s">
+      <c r="L4" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="93" t="s">
+      <c r="M4" s="87" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="104" t="s">
+      <c r="A5" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="76" t="s">
+      <c r="B5" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="76" t="s">
+      <c r="C5" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="57" t="s">
+      <c r="D5" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="86" t="s">
+      <c r="E5" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="87"/>
-      <c r="G5" s="96" t="s">
+      <c r="F5" s="81"/>
+      <c r="G5" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="97"/>
-      <c r="I5" s="100" t="s">
+      <c r="H5" s="91"/>
+      <c r="I5" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="102" t="s">
+      <c r="J5" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="98" t="s">
+      <c r="K5" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="91"/>
-      <c r="M5" s="94"/>
+      <c r="L5" s="85"/>
+      <c r="M5" s="88"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="105"/>
-      <c r="B6" s="77"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="58"/>
+      <c r="A6" s="99"/>
+      <c r="B6" s="101"/>
+      <c r="C6" s="101"/>
+      <c r="D6" s="68"/>
       <c r="E6" s="11" t="s">
         <v>21</v>
       </c>
@@ -2808,43 +2811,43 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="101"/>
-      <c r="J6" s="103"/>
-      <c r="K6" s="99"/>
-      <c r="L6" s="92"/>
-      <c r="M6" s="95"/>
+      <c r="I6" s="95"/>
+      <c r="J6" s="97"/>
+      <c r="K6" s="93"/>
+      <c r="L6" s="86"/>
+      <c r="M6" s="89"/>
     </row>
     <row r="7" spans="1:14" ht="88.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="70" t="s">
+      <c r="A7" s="105" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="44" t="s">
-        <v>162</v>
-      </c>
-      <c r="C7" s="44" t="s">
+      <c r="B7" s="43" t="s">
+        <v>161</v>
+      </c>
+      <c r="C7" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="44" t="s">
+      <c r="E7" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="44" t="s">
+      <c r="F7" s="43" t="s">
         <v>62</v>
       </c>
       <c r="G7" s="22" t="s">
         <v>65</v>
       </c>
       <c r="H7" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="K7" s="44"/>
-      <c r="L7" s="44" t="s">
+      <c r="K7" s="43"/>
+      <c r="L7" s="43" t="s">
         <v>38</v>
       </c>
       <c r="M7" s="24" t="s">
@@ -2852,54 +2855,54 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="71"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="44" t="s">
+      <c r="A8" s="106"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="H8" s="44" t="s">
-        <v>164</v>
-      </c>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="106" t="s">
+      <c r="H8" s="43" t="s">
+        <v>163</v>
+      </c>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="44"/>
+      <c r="M8" s="70" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="71"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="45"/>
-      <c r="K9" s="45"/>
-      <c r="L9" s="45"/>
-      <c r="M9" s="107"/>
+      <c r="A9" s="106"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="71"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="72"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="46"/>
-      <c r="K10" s="46"/>
-      <c r="L10" s="46"/>
+      <c r="A10" s="107"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="45"/>
       <c r="M10" s="31" t="s">
         <v>72</v>
       </c>
@@ -2908,33 +2911,33 @@
       <c r="A11" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="47" t="s">
+      <c r="C11" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="47" t="s">
+      <c r="D11" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="47" t="s">
+      <c r="E11" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="47" t="s">
+      <c r="F11" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="G11" s="47" t="s">
-        <v>165</v>
-      </c>
-      <c r="H11" s="47" t="s">
+      <c r="G11" s="58" t="s">
+        <v>164</v>
+      </c>
+      <c r="H11" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47" t="s">
+      <c r="I11" s="58"/>
+      <c r="J11" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="K11" s="47"/>
-      <c r="L11" s="47" t="s">
+      <c r="K11" s="58"/>
+      <c r="L11" s="58" t="s">
         <v>37</v>
       </c>
       <c r="M11" s="24" t="s">
@@ -2945,138 +2948,167 @@
       <c r="A12" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="49"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="49"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
       <c r="M12" s="32" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="86.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="103" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="C13" s="47" t="s">
+      <c r="C13" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="D13" s="47" t="s">
+      <c r="D13" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="E13" s="47" t="s">
+      <c r="E13" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="47" t="s">
+      <c r="F13" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="G13" s="44" t="s">
+      <c r="G13" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="H13" s="44" t="s">
+      <c r="H13" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47" t="s">
+      <c r="I13" s="58"/>
+      <c r="J13" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="K13" s="47"/>
-      <c r="L13" s="47" t="s">
+      <c r="K13" s="58"/>
+      <c r="L13" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="M13" s="47" t="s">
+      <c r="M13" s="58" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="98.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="75"/>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="49"/>
-      <c r="M14" s="49"/>
+      <c r="A14" s="104"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="60"/>
     </row>
     <row r="15" spans="1:14" ht="120.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="73" t="s">
-        <v>178</v>
-      </c>
-      <c r="C15" s="73" t="s">
+      <c r="B15" s="102" t="s">
+        <v>177</v>
+      </c>
+      <c r="C15" s="102" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="73" t="s">
+      <c r="D15" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="73" t="s">
+      <c r="E15" s="102" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="73" t="s">
+      <c r="F15" s="102" t="s">
         <v>74</v>
       </c>
-      <c r="G15" s="44" t="s">
-        <v>166</v>
-      </c>
-      <c r="H15" s="44" t="s">
+      <c r="G15" s="43" t="s">
+        <v>165</v>
+      </c>
+      <c r="H15" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="I15" s="73"/>
-      <c r="J15" s="73" t="s">
+      <c r="I15" s="102"/>
+      <c r="J15" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="K15" s="73"/>
-      <c r="L15" s="73" t="s">
+      <c r="K15" s="102"/>
+      <c r="L15" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="M15" s="73" t="s">
+      <c r="M15" s="102" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="73"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="73"/>
-      <c r="J16" s="73"/>
-      <c r="K16" s="73"/>
-      <c r="L16" s="73"/>
-      <c r="M16" s="73"/>
+      <c r="A16" s="102"/>
+      <c r="B16" s="102"/>
+      <c r="C16" s="102"/>
+      <c r="D16" s="102"/>
+      <c r="E16" s="102"/>
+      <c r="F16" s="102"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="102"/>
+      <c r="J16" s="102"/>
+      <c r="K16" s="102"/>
+      <c r="L16" s="102"/>
+      <c r="M16" s="102"/>
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="L7:L10"/>
-    <mergeCell ref="K7:K10"/>
-    <mergeCell ref="J7:J10"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I7:I10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="B7:B10"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="B3:M3"/>
@@ -3093,46 +3125,17 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I7:I10"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="L7:L10"/>
+    <mergeCell ref="K7:K10"/>
+    <mergeCell ref="J7:J10"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
@@ -3147,8 +3150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3D88CD-1BA6-4157-9522-8201A0FEDE3C}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13:H14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3175,83 +3178,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="69"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="57"/>
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="53" t="str">
+      <c r="B3" s="64" t="str">
         <f>'Listado Objetos de Dominio'!$B$6</f>
         <v xml:space="preserve"> Objeto de dominio que representa el Administrador encargado de hacer la creacion o gestión de las zonas comunes y la gestión de residentes y sus respectivas reservas en caso de ser necesario.</v>
       </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="54"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="65"/>
       <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="55"/>
+      <c r="C4" s="48"/>
       <c r="D4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="56"/>
-      <c r="G4" s="63" t="s">
+      <c r="F4" s="66"/>
+      <c r="G4" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="63"/>
+      <c r="H4" s="51"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -3261,52 +3264,52 @@
       <c r="K4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="66" t="s">
+      <c r="L4" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="67" t="s">
+      <c r="M4" s="55" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="57" t="s">
+      <c r="D5" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="56" t="s">
+      <c r="E5" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="56"/>
-      <c r="G5" s="61" t="s">
+      <c r="F5" s="66"/>
+      <c r="G5" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="61"/>
-      <c r="I5" s="64" t="s">
+      <c r="H5" s="49"/>
+      <c r="I5" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="65" t="s">
+      <c r="J5" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="62" t="s">
+      <c r="K5" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="66"/>
-      <c r="M5" s="67"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="55"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="60"/>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="58"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="68"/>
       <c r="E6" s="11" t="s">
         <v>21</v>
       </c>
@@ -3319,43 +3322,43 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="64"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="62"/>
-      <c r="L6" s="66"/>
-      <c r="M6" s="67"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="55"/>
     </row>
     <row r="7" spans="1:14" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="47" t="s">
+      <c r="D7" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="47" t="s">
+      <c r="E7" s="58" t="s">
         <v>79</v>
       </c>
-      <c r="F7" s="47" t="s">
+      <c r="F7" s="58" t="s">
         <v>80</v>
       </c>
       <c r="G7" s="34" t="s">
         <v>81</v>
       </c>
       <c r="H7" s="34" t="s">
-        <v>167</v>
-      </c>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47" t="s">
+        <v>166</v>
+      </c>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="47"/>
-      <c r="L7" s="47" t="s">
+      <c r="K7" s="58"/>
+      <c r="L7" s="58" t="s">
         <v>41</v>
       </c>
       <c r="M7" s="26" t="s">
@@ -3363,71 +3366,71 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="51"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="44" t="s">
-        <v>171</v>
-      </c>
-      <c r="H8" s="44" t="s">
-        <v>168</v>
-      </c>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="48"/>
+      <c r="A8" s="62"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="43" t="s">
+        <v>170</v>
+      </c>
+      <c r="H8" s="43" t="s">
+        <v>167</v>
+      </c>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="59"/>
+      <c r="L8" s="59"/>
       <c r="M8" s="26" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="51"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
+      <c r="A9" s="62"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="59"/>
       <c r="M9" s="108" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="51"/>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="48"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="48"/>
+      <c r="A10" s="62"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="59"/>
       <c r="M10" s="109"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="52"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="49"/>
-      <c r="K11" s="49"/>
-      <c r="L11" s="49"/>
+      <c r="A11" s="63"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="60"/>
       <c r="M11" s="110"/>
     </row>
     <row r="12" spans="1:14" ht="90" x14ac:dyDescent="0.25">
@@ -3450,10 +3453,10 @@
         <v>84</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I12" s="22"/>
       <c r="J12" s="22" t="s">
@@ -3471,33 +3474,33 @@
       <c r="A13" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="C13" s="47" t="s">
+      <c r="C13" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="D13" s="47" t="s">
+      <c r="D13" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="47" t="s">
+      <c r="E13" s="58" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="47" t="s">
+      <c r="F13" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="G13" s="73" t="s">
-        <v>173</v>
-      </c>
-      <c r="H13" s="73" t="s">
-        <v>191</v>
-      </c>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47" t="s">
+      <c r="G13" s="102" t="s">
+        <v>172</v>
+      </c>
+      <c r="H13" s="102" t="s">
+        <v>190</v>
+      </c>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="K13" s="47"/>
-      <c r="L13" s="47" t="s">
+      <c r="K13" s="58"/>
+      <c r="L13" s="58" t="s">
         <v>104</v>
       </c>
       <c r="M13" s="26" t="s">
@@ -3508,17 +3511,17 @@
       <c r="A14" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="73"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="49"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="102"/>
+      <c r="H14" s="102"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
       <c r="M14" s="30" t="s">
         <v>89</v>
       </c>
@@ -3528,7 +3531,7 @@
         <v>31</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>90</v>
@@ -3543,10 +3546,10 @@
         <v>84</v>
       </c>
       <c r="G15" s="22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H15" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I15" s="22"/>
       <c r="J15" s="22" t="s">
@@ -3565,6 +3568,31 @@
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L7:L11"/>
+    <mergeCell ref="K7:K11"/>
+    <mergeCell ref="J7:J11"/>
+    <mergeCell ref="I7:I11"/>
+    <mergeCell ref="G8:G11"/>
+    <mergeCell ref="H8:H11"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
     <mergeCell ref="M9:M11"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="A1:N1"/>
@@ -3581,31 +3609,6 @@
     <mergeCell ref="L4:L6"/>
     <mergeCell ref="M4:M6"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L7:L11"/>
-    <mergeCell ref="K7:K11"/>
-    <mergeCell ref="J7:J11"/>
-    <mergeCell ref="I7:I11"/>
-    <mergeCell ref="G8:G11"/>
-    <mergeCell ref="H8:H11"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="F7:F11"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="B7:B11"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
@@ -3651,84 +3654,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="78" t="str">
+      <c r="B2" s="72" t="str">
         <f>'Listado Objetos de Dominio'!A7</f>
         <v>ZonaInmueble</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="80"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="74"/>
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="81" t="str">
+      <c r="B3" s="75" t="str">
         <f>'Listado Objetos de Dominio'!B7</f>
         <v>Objeto de dominio que representa una Zona de Inmuebles en un conjunto residencial se refiere a una agrupación de unidades habitacionales (como una torre, bloque, o lote) que comparten una ubicación física y características comunes dentro del conjunto.</v>
       </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="83"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="77"/>
       <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="85"/>
+      <c r="C4" s="79"/>
       <c r="D4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="86" t="s">
+      <c r="E4" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="87"/>
-      <c r="G4" s="88" t="s">
+      <c r="F4" s="81"/>
+      <c r="G4" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="89"/>
+      <c r="H4" s="83"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -3738,52 +3741,52 @@
       <c r="K4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="90" t="s">
+      <c r="L4" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="93" t="s">
+      <c r="M4" s="87" t="s">
         <v>133</v>
       </c>
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="104" t="s">
+      <c r="A5" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="76" t="s">
+      <c r="B5" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="76" t="s">
+      <c r="C5" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="57" t="s">
+      <c r="D5" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="86" t="s">
+      <c r="E5" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="87"/>
-      <c r="G5" s="96" t="s">
+      <c r="F5" s="81"/>
+      <c r="G5" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="97"/>
-      <c r="I5" s="100" t="s">
+      <c r="H5" s="91"/>
+      <c r="I5" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="102" t="s">
+      <c r="J5" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="98" t="s">
+      <c r="K5" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="91"/>
-      <c r="M5" s="94"/>
+      <c r="L5" s="85"/>
+      <c r="M5" s="88"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="105"/>
-      <c r="B6" s="77"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="58"/>
+      <c r="A6" s="99"/>
+      <c r="B6" s="101"/>
+      <c r="C6" s="101"/>
+      <c r="D6" s="68"/>
       <c r="E6" s="11" t="s">
         <v>21</v>
       </c>
@@ -3796,43 +3799,43 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="101"/>
-      <c r="J6" s="103"/>
-      <c r="K6" s="99"/>
-      <c r="L6" s="92"/>
-      <c r="M6" s="95"/>
+      <c r="I6" s="95"/>
+      <c r="J6" s="97"/>
+      <c r="K6" s="93"/>
+      <c r="L6" s="86"/>
+      <c r="M6" s="89"/>
     </row>
     <row r="7" spans="1:14" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="73" t="s">
+      <c r="A7" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="73" t="s">
-        <v>175</v>
-      </c>
-      <c r="C7" s="73" t="s">
+      <c r="B7" s="102" t="s">
+        <v>174</v>
+      </c>
+      <c r="C7" s="102" t="s">
         <v>114</v>
       </c>
-      <c r="D7" s="73" t="s">
+      <c r="D7" s="102" t="s">
         <v>108</v>
       </c>
-      <c r="E7" s="73" t="s">
+      <c r="E7" s="102" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="73" t="s">
+      <c r="F7" s="102" t="s">
         <v>115</v>
       </c>
-      <c r="G7" s="73" t="s">
+      <c r="G7" s="102" t="s">
         <v>134</v>
       </c>
-      <c r="H7" s="73" t="s">
-        <v>190</v>
-      </c>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73" t="s">
+      <c r="H7" s="102" t="s">
+        <v>189</v>
+      </c>
+      <c r="I7" s="102"/>
+      <c r="J7" s="102" t="s">
         <v>116</v>
       </c>
-      <c r="K7" s="73"/>
-      <c r="L7" s="73" t="s">
+      <c r="K7" s="102"/>
+      <c r="L7" s="102" t="s">
         <v>117</v>
       </c>
       <c r="M7" s="22" t="s">
@@ -3840,35 +3843,35 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="73"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="73"/>
-      <c r="H8" s="73"/>
-      <c r="I8" s="73"/>
-      <c r="J8" s="73"/>
-      <c r="K8" s="73"/>
-      <c r="L8" s="73"/>
+      <c r="A8" s="102"/>
+      <c r="B8" s="102"/>
+      <c r="C8" s="102"/>
+      <c r="D8" s="102"/>
+      <c r="E8" s="102"/>
+      <c r="F8" s="102"/>
+      <c r="G8" s="102"/>
+      <c r="H8" s="102"/>
+      <c r="I8" s="102"/>
+      <c r="J8" s="102"/>
+      <c r="K8" s="102"/>
+      <c r="L8" s="102"/>
       <c r="M8" s="22" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="73"/>
-      <c r="B9" s="73"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="73"/>
-      <c r="J9" s="73"/>
-      <c r="K9" s="73"/>
-      <c r="L9" s="73"/>
+      <c r="A9" s="102"/>
+      <c r="B9" s="102"/>
+      <c r="C9" s="102"/>
+      <c r="D9" s="102"/>
+      <c r="E9" s="102"/>
+      <c r="F9" s="102"/>
+      <c r="G9" s="102"/>
+      <c r="H9" s="102"/>
+      <c r="I9" s="102"/>
+      <c r="J9" s="102"/>
+      <c r="K9" s="102"/>
+      <c r="L9" s="102"/>
       <c r="M9" s="22" t="s">
         <v>120</v>
       </c>
@@ -3877,33 +3880,33 @@
       <c r="A10" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="102" t="s">
         <v>121</v>
       </c>
-      <c r="C10" s="73" t="s">
+      <c r="C10" s="102" t="s">
         <v>122</v>
       </c>
-      <c r="D10" s="73" t="s">
+      <c r="D10" s="102" t="s">
         <v>108</v>
       </c>
-      <c r="E10" s="73" t="s">
+      <c r="E10" s="102" t="s">
         <v>63</v>
       </c>
-      <c r="F10" s="73" t="s">
+      <c r="F10" s="102" t="s">
         <v>123</v>
       </c>
-      <c r="G10" s="73" t="s">
-        <v>180</v>
-      </c>
-      <c r="H10" s="73" t="s">
-        <v>185</v>
-      </c>
-      <c r="I10" s="73"/>
-      <c r="J10" s="73" t="s">
+      <c r="G10" s="102" t="s">
+        <v>179</v>
+      </c>
+      <c r="H10" s="102" t="s">
+        <v>184</v>
+      </c>
+      <c r="I10" s="102"/>
+      <c r="J10" s="102" t="s">
         <v>124</v>
       </c>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73" t="s">
+      <c r="K10" s="102"/>
+      <c r="L10" s="102" t="s">
         <v>116</v>
       </c>
       <c r="M10" s="22" t="s">
@@ -3914,17 +3917,17 @@
       <c r="A11" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="73"/>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="73"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="73"/>
+      <c r="B11" s="102"/>
+      <c r="C11" s="102"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="102"/>
+      <c r="I11" s="102"/>
+      <c r="J11" s="102"/>
+      <c r="K11" s="102"/>
+      <c r="L11" s="102"/>
       <c r="M11" s="22" t="s">
         <v>120</v>
       </c>
@@ -3949,10 +3952,10 @@
         <v>126</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I12" s="22"/>
       <c r="J12" s="22" t="s">
@@ -3971,7 +3974,7 @@
         <v>31</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C13" s="22" t="s">
         <v>128</v>
@@ -3986,7 +3989,7 @@
         <v>129</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H13" s="22" t="s">
         <v>159</v>
@@ -4005,6 +4008,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
     <mergeCell ref="L10:L11"/>
     <mergeCell ref="L7:L9"/>
     <mergeCell ref="B10:B11"/>
@@ -4021,30 +4048,6 @@
     <mergeCell ref="K10:K11"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="I7:I9"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="K5:K6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{40DB47AD-DF64-4401-B17F-CC72FC22A8C4}"/>
@@ -4087,84 +4090,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="78" t="str">
+      <c r="B2" s="72" t="str">
         <f>'Listado Objetos de Dominio'!A7</f>
         <v>ZonaInmueble</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="80"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="74"/>
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="81" t="str">
+      <c r="B3" s="75" t="str">
         <f>'Listado Objetos de Dominio'!B7</f>
         <v>Objeto de dominio que representa una Zona de Inmuebles en un conjunto residencial se refiere a una agrupación de unidades habitacionales (como una torre, bloque, o lote) que comparten una ubicación física y características comunes dentro del conjunto.</v>
       </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="83"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="77"/>
       <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="85"/>
+      <c r="C4" s="79"/>
       <c r="D4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="86" t="s">
+      <c r="E4" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="87"/>
-      <c r="G4" s="88" t="s">
+      <c r="F4" s="81"/>
+      <c r="G4" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="89"/>
+      <c r="H4" s="83"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -4174,52 +4177,52 @@
       <c r="K4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="90" t="s">
+      <c r="L4" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="93" t="s">
+      <c r="M4" s="87" t="s">
         <v>133</v>
       </c>
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="104" t="s">
+      <c r="A5" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="76" t="s">
+      <c r="B5" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="76" t="s">
+      <c r="C5" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="57" t="s">
+      <c r="D5" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="86" t="s">
+      <c r="E5" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="87"/>
-      <c r="G5" s="96" t="s">
+      <c r="F5" s="81"/>
+      <c r="G5" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="97"/>
-      <c r="I5" s="100" t="s">
+      <c r="H5" s="91"/>
+      <c r="I5" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="102" t="s">
+      <c r="J5" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="98" t="s">
+      <c r="K5" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="91"/>
-      <c r="M5" s="94"/>
+      <c r="L5" s="85"/>
+      <c r="M5" s="88"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="105"/>
-      <c r="B6" s="77"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="58"/>
+      <c r="A6" s="99"/>
+      <c r="B6" s="101"/>
+      <c r="C6" s="101"/>
+      <c r="D6" s="68"/>
       <c r="E6" s="11" t="s">
         <v>21</v>
       </c>
@@ -4232,43 +4235,43 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="101"/>
-      <c r="J6" s="103"/>
-      <c r="K6" s="99"/>
-      <c r="L6" s="92"/>
-      <c r="M6" s="95"/>
+      <c r="I6" s="95"/>
+      <c r="J6" s="97"/>
+      <c r="K6" s="93"/>
+      <c r="L6" s="86"/>
+      <c r="M6" s="89"/>
     </row>
     <row r="7" spans="1:14" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="73" t="s">
+      <c r="A7" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="102" t="s">
         <v>141</v>
       </c>
-      <c r="C7" s="73" t="s">
+      <c r="C7" s="102" t="s">
         <v>142</v>
       </c>
-      <c r="D7" s="73" t="s">
+      <c r="D7" s="102" t="s">
         <v>109</v>
       </c>
-      <c r="E7" s="73" t="s">
+      <c r="E7" s="102" t="s">
         <v>151</v>
       </c>
-      <c r="F7" s="73" t="s">
+      <c r="F7" s="102" t="s">
         <v>152</v>
       </c>
-      <c r="G7" s="73" t="s">
+      <c r="G7" s="102" t="s">
         <v>157</v>
       </c>
-      <c r="H7" s="73" t="s">
-        <v>189</v>
-      </c>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73" t="s">
+      <c r="H7" s="102" t="s">
+        <v>188</v>
+      </c>
+      <c r="I7" s="102"/>
+      <c r="J7" s="102" t="s">
         <v>136</v>
       </c>
-      <c r="K7" s="73"/>
-      <c r="L7" s="73" t="s">
+      <c r="K7" s="102"/>
+      <c r="L7" s="102" t="s">
         <v>143</v>
       </c>
       <c r="M7" s="22" t="s">
@@ -4276,35 +4279,35 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="73"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="73"/>
-      <c r="H8" s="73"/>
-      <c r="I8" s="73"/>
-      <c r="J8" s="73"/>
-      <c r="K8" s="73"/>
-      <c r="L8" s="73"/>
+      <c r="A8" s="102"/>
+      <c r="B8" s="102"/>
+      <c r="C8" s="102"/>
+      <c r="D8" s="102"/>
+      <c r="E8" s="102"/>
+      <c r="F8" s="102"/>
+      <c r="G8" s="102"/>
+      <c r="H8" s="102"/>
+      <c r="I8" s="102"/>
+      <c r="J8" s="102"/>
+      <c r="K8" s="102"/>
+      <c r="L8" s="102"/>
       <c r="M8" s="22" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="73"/>
-      <c r="B9" s="73"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="73"/>
-      <c r="J9" s="73"/>
-      <c r="K9" s="73"/>
-      <c r="L9" s="73"/>
+      <c r="A9" s="102"/>
+      <c r="B9" s="102"/>
+      <c r="C9" s="102"/>
+      <c r="D9" s="102"/>
+      <c r="E9" s="102"/>
+      <c r="F9" s="102"/>
+      <c r="G9" s="102"/>
+      <c r="H9" s="102"/>
+      <c r="I9" s="102"/>
+      <c r="J9" s="102"/>
+      <c r="K9" s="102"/>
+      <c r="L9" s="102"/>
       <c r="M9" s="22" t="s">
         <v>146</v>
       </c>
@@ -4313,33 +4316,33 @@
       <c r="A10" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="102" t="s">
         <v>138</v>
       </c>
-      <c r="C10" s="73" t="s">
+      <c r="C10" s="102" t="s">
         <v>147</v>
       </c>
-      <c r="D10" s="73" t="s">
+      <c r="D10" s="102" t="s">
         <v>109</v>
       </c>
-      <c r="E10" s="73" t="s">
+      <c r="E10" s="102" t="s">
         <v>151</v>
       </c>
-      <c r="F10" s="73" t="s">
+      <c r="F10" s="102" t="s">
         <v>153</v>
       </c>
-      <c r="G10" s="73" t="s">
-        <v>186</v>
-      </c>
-      <c r="H10" s="73" t="s">
-        <v>184</v>
-      </c>
-      <c r="I10" s="73"/>
-      <c r="J10" s="73" t="s">
+      <c r="G10" s="102" t="s">
+        <v>185</v>
+      </c>
+      <c r="H10" s="102" t="s">
+        <v>183</v>
+      </c>
+      <c r="I10" s="102"/>
+      <c r="J10" s="102" t="s">
         <v>139</v>
       </c>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73" t="s">
+      <c r="K10" s="102"/>
+      <c r="L10" s="102" t="s">
         <v>135</v>
       </c>
       <c r="M10" s="22" t="s">
@@ -4350,17 +4353,17 @@
       <c r="A11" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="73"/>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="73"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="73"/>
+      <c r="B11" s="102"/>
+      <c r="C11" s="102"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="102"/>
+      <c r="I11" s="102"/>
+      <c r="J11" s="102"/>
+      <c r="K11" s="102"/>
+      <c r="L11" s="102"/>
       <c r="M11" s="22" t="s">
         <v>146</v>
       </c>
@@ -4385,7 +4388,7 @@
         <v>154</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H12" s="22" t="s">
         <v>159</v>
@@ -4422,10 +4425,10 @@
         <v>156</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I13" s="22"/>
       <c r="J13" s="22" t="s">
@@ -4441,18 +4444,18 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="L7:L9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="K5:K6"/>
@@ -4469,18 +4472,18 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="L7:L9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{DE0AC091-170B-4F28-806F-0CE19EF466E0}"/>
@@ -4497,6 +4500,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C279D002CEC08F42B7087C30E58D0266" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e5713f579c7011938dc4987ae8981b8f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3219184d-29ab-4105-b29c-8e343e335d59" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae0a0ff84a3c6712467f60982d6e378d" ns2:_="">
     <xsd:import namespace="3219184d-29ab-4105-b29c-8e343e335d59"/>
@@ -4640,15 +4652,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2038022-656B-4A1B-A485-51A1972238BD}">
   <ds:schemaRefs>
@@ -4667,6 +4670,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6724C681-8A04-4D66-BB1C-57F7466573C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AEECCE0-61F9-4782-94C5-382F8EFF459D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4684,14 +4695,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6724C681-8A04-4D66-BB1C-57F7466573C0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{6ebbfa72-b3b6-4c1f-8b23-058d4f67f013}" enabled="1" method="Privileged" siteId="{bf1ce8b5-5d39-4bc5-ad6e-07b3e4d7d67a}" contentBits="0" removed="0"/>

</xml_diff>

<commit_message>
Realice las responsabilidades de zona inmueble e inmueble ademas de corregir ciertos aspectos en el documento conjuntos residenciales de dominio enriquesido
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/Event Storming/ConjuntosResidenciales - Event Storming.xlsx
+++ b/Doo-Doc/Nueva Version Victus/Event Storming/ConjuntosResidenciales - Event Storming.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Music\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josez\Documents\Universidad IngeSistemas\Diseño Orientado a Objetos(DOO)\VictusProyect\victus-doc\Doo-Doc\Nueva Version Victus\Event Storming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6E5A14-D0A0-4C9B-9844-340D68CAD301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A101F4B0-905C-483F-91BD-C56AB6A65D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="2" activeTab="4" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="3" activeTab="5" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
   </bookViews>
   <sheets>
     <sheet name="Flujo de eventos en el tiempo" sheetId="61" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="195">
   <si>
     <t>Descripción</t>
   </si>
@@ -570,9 +570,6 @@
   </si>
   <si>
     <t>Registrar zona inmueble</t>
-  </si>
-  <si>
-    <t>Dar de baja zona inmueble</t>
   </si>
   <si>
     <t>Dar de baja administrador</t>
@@ -1266,6 +1263,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1275,15 +1275,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1311,154 +1338,124 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1869,15 +1866,15 @@
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="2"/>
+    <col min="1" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1"/>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F18"/>
     </row>
   </sheetData>
@@ -1896,15 +1893,15 @@
       <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>27</v>
       </c>
@@ -1914,7 +1911,7 @@
       <c r="C1" s="37"/>
       <c r="D1" s="38"/>
     </row>
-    <row r="2" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>28</v>
       </c>
@@ -1924,7 +1921,7 @@
       <c r="C2" s="40"/>
       <c r="D2" s="41"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>4</v>
       </c>
@@ -1938,7 +1935,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="73.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="28" t="s">
         <v>29</v>
       </c>
@@ -1953,7 +1950,7 @@
         <v>Conjuntos reisdenciales</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="28" t="s">
         <v>30</v>
       </c>
@@ -1965,7 +1962,7 @@
       </c>
       <c r="D5" s="42"/>
     </row>
-    <row r="6" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="28" t="s">
         <v>31</v>
       </c>
@@ -1977,7 +1974,7 @@
       </c>
       <c r="D6" s="42"/>
     </row>
-    <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="28" t="s">
         <v>108</v>
       </c>
@@ -1989,7 +1986,7 @@
       </c>
       <c r="D7" s="42"/>
     </row>
-    <row r="8" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="28" t="s">
         <v>109</v>
       </c>
@@ -2027,107 +2024,107 @@
       <selection activeCell="H7" sqref="H7:H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="18.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="36.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="36.109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="28.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="1"/>
+    <col min="13" max="13" width="46.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="57"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="67"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="64" t="str">
+      <c r="B3" s="68" t="str">
         <f>'Listado Objetos de Dominio'!B4</f>
         <v>Objeto de dominio que representa cada una de las comunidades habitacionales organizadas en un sistema. Abarca la totalidad de los elementos que componen el conjunto, desde las unidades habitacionales individuales (inmuebles) hasta las zonas comunes.</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="65"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="69"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="48"/>
+      <c r="C4" s="53"/>
       <c r="D4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="66" t="s">
+      <c r="E4" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="66"/>
-      <c r="G4" s="51" t="s">
+      <c r="F4" s="54"/>
+      <c r="G4" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="51"/>
+      <c r="H4" s="61"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -2137,52 +2134,52 @@
       <c r="K4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="54" t="s">
+      <c r="L4" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="55" t="s">
+      <c r="M4" s="65" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="67" t="s">
+      <c r="D5" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="66" t="s">
+      <c r="E5" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="66"/>
-      <c r="G5" s="49" t="s">
+      <c r="F5" s="54"/>
+      <c r="G5" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="49"/>
-      <c r="I5" s="52" t="s">
+      <c r="H5" s="59"/>
+      <c r="I5" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="53" t="s">
+      <c r="J5" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="50" t="s">
+      <c r="K5" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="54"/>
-      <c r="M5" s="55"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="68"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="65"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="58"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="56"/>
       <c r="E6" s="11" t="s">
         <v>21</v>
       </c>
@@ -2195,221 +2192,221 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="52"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="55"/>
-    </row>
-    <row r="7" spans="1:14" ht="87.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="61" t="s">
+      <c r="I6" s="62"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="65"/>
+    </row>
+    <row r="7" spans="1:14" ht="87.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="58" t="s">
+      <c r="D7" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="43" t="s">
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="43" t="s">
+      <c r="H7" s="44" t="s">
         <v>158</v>
       </c>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58" t="s">
+      <c r="I7" s="47"/>
+      <c r="J7" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="K7" s="58"/>
-      <c r="L7" s="58" t="s">
+      <c r="K7" s="47"/>
+      <c r="L7" s="47" t="s">
         <v>36</v>
       </c>
       <c r="M7" s="26" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="62"/>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="59"/>
-      <c r="J8" s="59"/>
-      <c r="K8" s="59"/>
-      <c r="L8" s="59"/>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="51"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="48"/>
       <c r="M8" s="26" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="62"/>
-      <c r="B9" s="59"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="59"/>
-      <c r="K9" s="59"/>
-      <c r="L9" s="59"/>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="51"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="48"/>
       <c r="M9" s="26" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="62"/>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="69" t="s">
+    <row r="10" spans="1:14" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="51"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="H10" s="69" t="s">
+      <c r="H10" s="43" t="s">
         <v>160</v>
       </c>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="59"/>
-      <c r="L10" s="59"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
       <c r="M10" s="26" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="63"/>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="60"/>
-      <c r="K11" s="60"/>
-      <c r="L11" s="60"/>
+    <row r="11" spans="1:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="52"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
       <c r="M11" s="26" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="61" t="s">
+    <row r="12" spans="1:14" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="58" t="s">
+      <c r="C12" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="58" t="s">
+      <c r="D12" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="58"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="43" t="s">
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="H12" s="43" t="s">
+      <c r="H12" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="I12" s="58"/>
-      <c r="J12" s="58" t="s">
+      <c r="I12" s="47"/>
+      <c r="J12" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="K12" s="58"/>
-      <c r="L12" s="58" t="s">
+      <c r="K12" s="47"/>
+      <c r="L12" s="47" t="s">
         <v>44</v>
       </c>
       <c r="M12" s="26" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="62"/>
-      <c r="B13" s="59"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
+    <row r="13" spans="1:14" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="51"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
       <c r="M13" s="26" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="62"/>
-      <c r="B14" s="59"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="59"/>
-      <c r="J14" s="59"/>
-      <c r="K14" s="59"/>
-      <c r="L14" s="59"/>
+    <row r="14" spans="1:14" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="51"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="48"/>
+      <c r="L14" s="48"/>
       <c r="M14" s="26" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="63"/>
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="60"/>
-      <c r="L15" s="60"/>
+    <row r="15" spans="1:14" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="52"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="49"/>
       <c r="M15" s="26" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="36" t="s">
         <v>45</v>
       </c>
       <c r="B16" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="C16" s="35" t="s">
         <v>191</v>
-      </c>
-      <c r="C16" s="35" t="s">
-        <v>192</v>
       </c>
       <c r="D16" s="35" t="s">
         <v>29</v>
       </c>
       <c r="E16" s="35"/>
       <c r="F16" s="35"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
       <c r="I16" s="35"/>
       <c r="J16" s="35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K16" s="35"/>
       <c r="L16" s="35" t="s">
@@ -2419,7 +2416,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="99.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="25" t="s">
         <v>52</v>
       </c>
@@ -2434,10 +2431,10 @@
       </c>
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
-      <c r="G17" s="69" t="s">
-        <v>194</v>
-      </c>
-      <c r="H17" s="69" t="s">
+      <c r="G17" s="43" t="s">
+        <v>193</v>
+      </c>
+      <c r="H17" s="43" t="s">
         <v>160</v>
       </c>
       <c r="I17" s="22"/>
@@ -2452,7 +2449,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
         <v>45</v>
       </c>
@@ -2467,8 +2464,8 @@
       </c>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
-      <c r="G18" s="69"/>
-      <c r="H18" s="69"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
       <c r="I18" s="22"/>
       <c r="J18" s="22" t="s">
         <v>34</v>
@@ -2481,7 +2478,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="25" t="s">
         <v>31</v>
       </c>
@@ -2496,10 +2493,10 @@
       </c>
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
-      <c r="G19" s="43" t="s">
-        <v>195</v>
-      </c>
-      <c r="H19" s="43" t="s">
+      <c r="G19" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="H19" s="44" t="s">
         <v>159</v>
       </c>
       <c r="I19" s="22"/>
@@ -2514,7 +2511,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="25" t="s">
         <v>31</v>
       </c>
@@ -2529,8 +2526,8 @@
       </c>
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="45"/>
       <c r="I20" s="22"/>
       <c r="J20" s="22" t="s">
         <v>41</v>
@@ -2543,12 +2540,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="25" t="s">
         <v>45</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C21" s="22" t="s">
         <v>61</v>
@@ -2558,8 +2555,8 @@
       </c>
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
       <c r="I21" s="22"/>
       <c r="J21" s="22" t="s">
         <v>36</v>
@@ -2574,37 +2571,6 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="G12:G16"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="G19:G21"/>
-    <mergeCell ref="H19:H21"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="F12:F15"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="L12:L15"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="I12:I15"/>
-    <mergeCell ref="H12:H16"/>
-    <mergeCell ref="L7:L11"/>
-    <mergeCell ref="K7:K11"/>
-    <mergeCell ref="J7:J11"/>
-    <mergeCell ref="I7:I11"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="F7:F11"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="C7:C11"/>
     <mergeCell ref="G7:G9"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A5:A6"/>
@@ -2621,6 +2587,37 @@
     <mergeCell ref="B7:B11"/>
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="L7:L11"/>
+    <mergeCell ref="K7:K11"/>
+    <mergeCell ref="J7:J11"/>
+    <mergeCell ref="I7:I11"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="L12:L15"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="I12:I15"/>
+    <mergeCell ref="H12:H16"/>
+    <mergeCell ref="G19:G21"/>
+    <mergeCell ref="H19:H21"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="G12:G16"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:H18"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
@@ -2642,108 +2639,108 @@
       <selection pane="bottomLeft" activeCell="C13" sqref="C13:C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="31" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="37.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="37.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="1"/>
+    <col min="13" max="13" width="46.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="74"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="80"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="75" t="str">
+      <c r="B3" s="81" t="str">
         <f>'Listado Objetos de Dominio'!$B$5</f>
         <v>Objeto de dominio que representa a cada una de las zonas comunes que se encuentran dentro de un conjunto residencial para que los residentes puedan reservar esos espacios y porder usarlos.</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
-      <c r="M3" s="77"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="83"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="79"/>
+      <c r="C4" s="85"/>
       <c r="D4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="80" t="s">
+      <c r="E4" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="81"/>
-      <c r="G4" s="82" t="s">
+      <c r="F4" s="87"/>
+      <c r="G4" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="83"/>
+      <c r="H4" s="89"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -2753,52 +2750,52 @@
       <c r="K4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="84" t="s">
+      <c r="L4" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="87" t="s">
+      <c r="M4" s="93" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="98" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="100" t="s">
+      <c r="B5" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="100" t="s">
+      <c r="C5" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="67" t="s">
+      <c r="D5" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="80" t="s">
+      <c r="E5" s="86" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="81"/>
-      <c r="G5" s="90" t="s">
+      <c r="F5" s="87"/>
+      <c r="G5" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="91"/>
-      <c r="I5" s="94" t="s">
+      <c r="H5" s="97"/>
+      <c r="I5" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="96" t="s">
+      <c r="J5" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="92" t="s">
+      <c r="K5" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="85"/>
-      <c r="M5" s="88"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="99"/>
-      <c r="B6" s="101"/>
-      <c r="C6" s="101"/>
-      <c r="D6" s="68"/>
+      <c r="L5" s="91"/>
+      <c r="M5" s="94"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="105"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="56"/>
       <c r="E6" s="11" t="s">
         <v>21</v>
       </c>
@@ -2811,29 +2808,29 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="95"/>
-      <c r="J6" s="97"/>
-      <c r="K6" s="93"/>
-      <c r="L6" s="86"/>
-      <c r="M6" s="89"/>
-    </row>
-    <row r="7" spans="1:14" ht="88.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="105" t="s">
+      <c r="I6" s="101"/>
+      <c r="J6" s="103"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="92"/>
+      <c r="M6" s="95"/>
+    </row>
+    <row r="7" spans="1:14" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="44" t="s">
         <v>161</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="43" t="s">
+      <c r="F7" s="44" t="s">
         <v>62</v>
       </c>
       <c r="G7" s="22" t="s">
@@ -2842,238 +2839,279 @@
       <c r="H7" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43" t="s">
+      <c r="I7" s="44"/>
+      <c r="J7" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43" t="s">
+      <c r="K7" s="44"/>
+      <c r="L7" s="44" t="s">
         <v>38</v>
       </c>
       <c r="M7" s="24" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="106"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="43" t="s">
+    <row r="8" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="71"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="H8" s="43" t="s">
+      <c r="H8" s="44" t="s">
         <v>163</v>
       </c>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
-      <c r="M8" s="70" t="s">
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
+      <c r="M8" s="106" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="106"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="71"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="107"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="45"/>
-      <c r="K10" s="45"/>
-      <c r="L10" s="45"/>
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="71"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="45"/>
+      <c r="K9" s="45"/>
+      <c r="L9" s="45"/>
+      <c r="M9" s="107"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="72"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="46"/>
       <c r="M10" s="31" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="58" t="s">
+      <c r="C11" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="58" t="s">
+      <c r="D11" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="58" t="s">
+      <c r="E11" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="58" t="s">
+      <c r="F11" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="G11" s="58" t="s">
+      <c r="G11" s="47" t="s">
         <v>164</v>
       </c>
-      <c r="H11" s="58" t="s">
+      <c r="H11" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="I11" s="58"/>
-      <c r="J11" s="58" t="s">
+      <c r="I11" s="47"/>
+      <c r="J11" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="K11" s="58"/>
-      <c r="L11" s="58" t="s">
+      <c r="K11" s="47"/>
+      <c r="L11" s="47" t="s">
         <v>37</v>
       </c>
       <c r="M11" s="24" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="60"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="60"/>
-      <c r="L12" s="60"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="49"/>
       <c r="M12" s="32" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="86.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="103" t="s">
+    <row r="13" spans="1:14" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="C13" s="58" t="s">
+      <c r="C13" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="D13" s="58" t="s">
+      <c r="D13" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="E13" s="58" t="s">
+      <c r="E13" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="58" t="s">
+      <c r="F13" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="G13" s="43" t="s">
+      <c r="G13" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="H13" s="43" t="s">
+      <c r="H13" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="I13" s="58"/>
-      <c r="J13" s="58" t="s">
+      <c r="I13" s="47"/>
+      <c r="J13" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="K13" s="58"/>
-      <c r="L13" s="58" t="s">
+      <c r="K13" s="47"/>
+      <c r="L13" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="M13" s="58" t="s">
+      <c r="M13" s="47" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="98.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="104"/>
-      <c r="B14" s="60"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="60"/>
-      <c r="L14" s="60"/>
-      <c r="M14" s="60"/>
-    </row>
-    <row r="15" spans="1:14" ht="120.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="102" t="s">
+    <row r="14" spans="1:14" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="75"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="49"/>
+    </row>
+    <row r="15" spans="1:14" ht="120.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="102" t="s">
-        <v>177</v>
-      </c>
-      <c r="C15" s="102" t="s">
+      <c r="B15" s="73" t="s">
+        <v>176</v>
+      </c>
+      <c r="C15" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="102" t="s">
+      <c r="D15" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="102" t="s">
+      <c r="E15" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="102" t="s">
+      <c r="F15" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="G15" s="43" t="s">
+      <c r="G15" s="44" t="s">
         <v>165</v>
       </c>
-      <c r="H15" s="43" t="s">
+      <c r="H15" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="I15" s="102"/>
-      <c r="J15" s="102" t="s">
+      <c r="I15" s="73"/>
+      <c r="J15" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="K15" s="102"/>
-      <c r="L15" s="102" t="s">
+      <c r="K15" s="73"/>
+      <c r="L15" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="M15" s="102" t="s">
+      <c r="M15" s="73" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="102"/>
-      <c r="B16" s="102"/>
-      <c r="C16" s="102"/>
-      <c r="D16" s="102"/>
-      <c r="E16" s="102"/>
-      <c r="F16" s="102"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="102"/>
-      <c r="J16" s="102"/>
-      <c r="K16" s="102"/>
-      <c r="L16" s="102"/>
-      <c r="M16" s="102"/>
+    <row r="16" spans="1:14" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="73"/>
+      <c r="B16" s="73"/>
+      <c r="C16" s="73"/>
+      <c r="D16" s="73"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="73"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="73"/>
+      <c r="J16" s="73"/>
+      <c r="K16" s="73"/>
+      <c r="L16" s="73"/>
+      <c r="M16" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="L7:L10"/>
+    <mergeCell ref="K7:K10"/>
+    <mergeCell ref="J7:J10"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I7:I10"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
     <mergeCell ref="K15:K16"/>
     <mergeCell ref="L15:L16"/>
     <mergeCell ref="M15:M16"/>
@@ -3090,52 +3128,11 @@
     <mergeCell ref="M13:M14"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I7:I10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="L7:L10"/>
-    <mergeCell ref="K7:K10"/>
-    <mergeCell ref="J7:J10"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="C7:C10"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
@@ -3150,111 +3147,111 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3D88CD-1BA6-4157-9522-8201A0FEDE3C}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="18.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="31.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="43.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="31.5546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="43.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="1"/>
+    <col min="13" max="13" width="46.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="57"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="67"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="64" t="str">
+      <c r="B3" s="68" t="str">
         <f>'Listado Objetos de Dominio'!$B$6</f>
         <v xml:space="preserve"> Objeto de dominio que representa el Administrador encargado de hacer la creacion o gestión de las zonas comunes y la gestión de residentes y sus respectivas reservas en caso de ser necesario.</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="65"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="69"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="48"/>
+      <c r="C4" s="53"/>
       <c r="D4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="66" t="s">
+      <c r="E4" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="66"/>
-      <c r="G4" s="51" t="s">
+      <c r="F4" s="54"/>
+      <c r="G4" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="51"/>
+      <c r="H4" s="61"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -3264,52 +3261,52 @@
       <c r="K4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="54" t="s">
+      <c r="L4" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="55" t="s">
+      <c r="M4" s="65" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="67" t="s">
+      <c r="D5" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="66" t="s">
+      <c r="E5" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="66"/>
-      <c r="G5" s="49" t="s">
+      <c r="F5" s="54"/>
+      <c r="G5" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="49"/>
-      <c r="I5" s="52" t="s">
+      <c r="H5" s="59"/>
+      <c r="I5" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="53" t="s">
+      <c r="J5" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="50" t="s">
+      <c r="K5" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="54"/>
-      <c r="M5" s="55"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="68"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="65"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="58"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="56"/>
       <c r="E6" s="11" t="s">
         <v>21</v>
       </c>
@@ -3322,29 +3319,29 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="52"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="55"/>
-    </row>
-    <row r="7" spans="1:14" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="61" t="s">
+      <c r="I6" s="62"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="65"/>
+    </row>
+    <row r="7" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="58" t="s">
+      <c r="D7" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="58" t="s">
+      <c r="E7" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="F7" s="58" t="s">
+      <c r="F7" s="47" t="s">
         <v>80</v>
       </c>
       <c r="G7" s="34" t="s">
@@ -3353,87 +3350,87 @@
       <c r="H7" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58" t="s">
+      <c r="I7" s="47"/>
+      <c r="J7" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="58"/>
-      <c r="L7" s="58" t="s">
+      <c r="K7" s="47"/>
+      <c r="L7" s="47" t="s">
         <v>41</v>
       </c>
       <c r="M7" s="26" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="62"/>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="43" t="s">
+    <row r="8" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="51"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="44" t="s">
         <v>170</v>
       </c>
-      <c r="H8" s="43" t="s">
+      <c r="H8" s="44" t="s">
         <v>167</v>
       </c>
-      <c r="I8" s="59"/>
-      <c r="J8" s="59"/>
-      <c r="K8" s="59"/>
-      <c r="L8" s="59"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="48"/>
       <c r="M8" s="26" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="62"/>
-      <c r="B9" s="59"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="59"/>
-      <c r="K9" s="59"/>
-      <c r="L9" s="59"/>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="51"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="48"/>
       <c r="M9" s="108" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="62"/>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="59"/>
-      <c r="L10" s="59"/>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="51"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
       <c r="M10" s="109"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="63"/>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="60"/>
-      <c r="K11" s="60"/>
-      <c r="L11" s="60"/>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="52"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
       <c r="M11" s="110"/>
     </row>
-    <row r="12" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
         <v>31</v>
       </c>
@@ -3470,68 +3467,68 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="C13" s="58" t="s">
+      <c r="C13" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="D13" s="58" t="s">
+      <c r="D13" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="58" t="s">
+      <c r="E13" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="58" t="s">
+      <c r="F13" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="G13" s="102" t="s">
+      <c r="G13" s="73" t="s">
         <v>172</v>
       </c>
-      <c r="H13" s="102" t="s">
-        <v>190</v>
-      </c>
-      <c r="I13" s="58"/>
-      <c r="J13" s="58" t="s">
+      <c r="H13" s="73" t="s">
+        <v>189</v>
+      </c>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="K13" s="58"/>
-      <c r="L13" s="58" t="s">
+      <c r="K13" s="47"/>
+      <c r="L13" s="47" t="s">
         <v>104</v>
       </c>
       <c r="M13" s="26" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="60"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="102"/>
-      <c r="H14" s="102"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="60"/>
-      <c r="L14" s="60"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="73"/>
+      <c r="H14" s="73"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="49"/>
       <c r="M14" s="30" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="25" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>90</v>
@@ -3563,36 +3560,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E16" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="F7:F11"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L7:L11"/>
-    <mergeCell ref="K7:K11"/>
-    <mergeCell ref="J7:J11"/>
-    <mergeCell ref="I7:I11"/>
-    <mergeCell ref="G8:G11"/>
-    <mergeCell ref="H8:H11"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
     <mergeCell ref="M9:M11"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="A1:N1"/>
@@ -3609,6 +3581,31 @@
     <mergeCell ref="L4:L6"/>
     <mergeCell ref="M4:M6"/>
     <mergeCell ref="E5:F5"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L7:L11"/>
+    <mergeCell ref="K7:K11"/>
+    <mergeCell ref="J7:J11"/>
+    <mergeCell ref="I7:I11"/>
+    <mergeCell ref="G8:G11"/>
+    <mergeCell ref="H8:H11"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="B7:B11"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
@@ -3625,113 +3622,113 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB345C48-C8D9-4186-9152-4D78F60A6B79}">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="29" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="37.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="37.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="1"/>
+    <col min="13" max="13" width="46.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="72" t="str">
+      <c r="B2" s="78" t="str">
         <f>'Listado Objetos de Dominio'!A7</f>
         <v>ZonaInmueble</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="74"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="80"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="75" t="str">
+      <c r="B3" s="81" t="str">
         <f>'Listado Objetos de Dominio'!B7</f>
         <v>Objeto de dominio que representa una Zona de Inmuebles en un conjunto residencial se refiere a una agrupación de unidades habitacionales (como una torre, bloque, o lote) que comparten una ubicación física y características comunes dentro del conjunto.</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
-      <c r="M3" s="77"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="83"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="84" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="79"/>
+      <c r="C4" s="85"/>
       <c r="D4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="80" t="s">
+      <c r="E4" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="81"/>
-      <c r="G4" s="82" t="s">
+      <c r="F4" s="87"/>
+      <c r="G4" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="83"/>
+      <c r="H4" s="89"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -3741,52 +3738,52 @@
       <c r="K4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="84" t="s">
+      <c r="L4" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="87" t="s">
+      <c r="M4" s="93" t="s">
         <v>133</v>
       </c>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="98" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="100" t="s">
+      <c r="B5" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="100" t="s">
+      <c r="C5" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="67" t="s">
+      <c r="D5" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="80" t="s">
+      <c r="E5" s="86" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="81"/>
-      <c r="G5" s="90" t="s">
+      <c r="F5" s="87"/>
+      <c r="G5" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="91"/>
-      <c r="I5" s="94" t="s">
+      <c r="H5" s="97"/>
+      <c r="I5" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="96" t="s">
+      <c r="J5" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="92" t="s">
+      <c r="K5" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="85"/>
-      <c r="M5" s="88"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="99"/>
-      <c r="B6" s="101"/>
-      <c r="C6" s="101"/>
-      <c r="D6" s="68"/>
+      <c r="L5" s="91"/>
+      <c r="M5" s="94"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="105"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="56"/>
       <c r="E6" s="11" t="s">
         <v>21</v>
       </c>
@@ -3799,140 +3796,140 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="95"/>
-      <c r="J6" s="97"/>
-      <c r="K6" s="93"/>
-      <c r="L6" s="86"/>
-      <c r="M6" s="89"/>
-    </row>
-    <row r="7" spans="1:14" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="102" t="s">
+      <c r="I6" s="101"/>
+      <c r="J6" s="103"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="92"/>
+      <c r="M6" s="95"/>
+    </row>
+    <row r="7" spans="1:14" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="102" t="s">
+      <c r="B7" s="73" t="s">
         <v>174</v>
       </c>
-      <c r="C7" s="102" t="s">
+      <c r="C7" s="73" t="s">
         <v>114</v>
       </c>
-      <c r="D7" s="102" t="s">
+      <c r="D7" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="E7" s="102" t="s">
+      <c r="E7" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="102" t="s">
+      <c r="F7" s="73" t="s">
         <v>115</v>
       </c>
-      <c r="G7" s="102" t="s">
+      <c r="G7" s="73" t="s">
         <v>134</v>
       </c>
-      <c r="H7" s="102" t="s">
-        <v>189</v>
-      </c>
-      <c r="I7" s="102"/>
-      <c r="J7" s="102" t="s">
+      <c r="H7" s="73" t="s">
+        <v>188</v>
+      </c>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73" t="s">
         <v>116</v>
       </c>
-      <c r="K7" s="102"/>
-      <c r="L7" s="102" t="s">
+      <c r="K7" s="73"/>
+      <c r="L7" s="73" t="s">
         <v>117</v>
       </c>
       <c r="M7" s="22" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="102"/>
-      <c r="B8" s="102"/>
-      <c r="C8" s="102"/>
-      <c r="D8" s="102"/>
-      <c r="E8" s="102"/>
-      <c r="F8" s="102"/>
-      <c r="G8" s="102"/>
-      <c r="H8" s="102"/>
-      <c r="I8" s="102"/>
-      <c r="J8" s="102"/>
-      <c r="K8" s="102"/>
-      <c r="L8" s="102"/>
+    <row r="8" spans="1:14" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="73"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="73"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="73"/>
       <c r="M8" s="22" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="102"/>
-      <c r="B9" s="102"/>
-      <c r="C9" s="102"/>
-      <c r="D9" s="102"/>
-      <c r="E9" s="102"/>
-      <c r="F9" s="102"/>
-      <c r="G9" s="102"/>
-      <c r="H9" s="102"/>
-      <c r="I9" s="102"/>
-      <c r="J9" s="102"/>
-      <c r="K9" s="102"/>
-      <c r="L9" s="102"/>
+    <row r="9" spans="1:14" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="73"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="73"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
       <c r="M9" s="22" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="102" t="s">
+      <c r="B10" s="73" t="s">
         <v>121</v>
       </c>
-      <c r="C10" s="102" t="s">
+      <c r="C10" s="73" t="s">
         <v>122</v>
       </c>
-      <c r="D10" s="102" t="s">
+      <c r="D10" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="E10" s="102" t="s">
+      <c r="E10" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="F10" s="102" t="s">
+      <c r="F10" s="73" t="s">
         <v>123</v>
       </c>
-      <c r="G10" s="102" t="s">
-        <v>179</v>
-      </c>
-      <c r="H10" s="102" t="s">
-        <v>184</v>
-      </c>
-      <c r="I10" s="102"/>
-      <c r="J10" s="102" t="s">
+      <c r="G10" s="73" t="s">
+        <v>178</v>
+      </c>
+      <c r="H10" s="73" t="s">
+        <v>183</v>
+      </c>
+      <c r="I10" s="73"/>
+      <c r="J10" s="73" t="s">
         <v>124</v>
       </c>
-      <c r="K10" s="102"/>
-      <c r="L10" s="102" t="s">
+      <c r="K10" s="73"/>
+      <c r="L10" s="73" t="s">
         <v>116</v>
       </c>
       <c r="M10" s="22" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="102"/>
-      <c r="C11" s="102"/>
-      <c r="D11" s="102"/>
-      <c r="E11" s="102"/>
-      <c r="F11" s="102"/>
-      <c r="G11" s="102"/>
-      <c r="H11" s="102"/>
-      <c r="I11" s="102"/>
-      <c r="J11" s="102"/>
-      <c r="K11" s="102"/>
-      <c r="L11" s="102"/>
+      <c r="B11" s="73"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="73"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="73"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="73"/>
       <c r="M11" s="22" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="105.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="105.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>31</v>
       </c>
@@ -3952,10 +3949,10 @@
         <v>126</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I12" s="22"/>
       <c r="J12" s="22" t="s">
@@ -3969,12 +3966,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="120.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="120.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
         <v>31</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>175</v>
+        <v>120</v>
       </c>
       <c r="C13" s="22" t="s">
         <v>128</v>
@@ -3989,7 +3986,7 @@
         <v>129</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H13" s="22" t="s">
         <v>159</v>
@@ -4008,30 +4005,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
     <mergeCell ref="L10:L11"/>
     <mergeCell ref="L7:L9"/>
     <mergeCell ref="B10:B11"/>
@@ -4048,6 +4021,30 @@
     <mergeCell ref="K10:K11"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="I7:I9"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="K5:K6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{40DB47AD-DF64-4401-B17F-CC72FC22A8C4}"/>
@@ -4065,109 +4062,109 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="37.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="37.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="1"/>
+    <col min="13" max="13" width="46.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="72" t="str">
+      <c r="B2" s="78" t="str">
         <f>'Listado Objetos de Dominio'!A7</f>
         <v>ZonaInmueble</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="74"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="80"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="75" t="str">
+      <c r="B3" s="81" t="str">
         <f>'Listado Objetos de Dominio'!B7</f>
         <v>Objeto de dominio que representa una Zona de Inmuebles en un conjunto residencial se refiere a una agrupación de unidades habitacionales (como una torre, bloque, o lote) que comparten una ubicación física y características comunes dentro del conjunto.</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
-      <c r="M3" s="77"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="83"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="84" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="79"/>
+      <c r="C4" s="85"/>
       <c r="D4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="80" t="s">
+      <c r="E4" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="81"/>
-      <c r="G4" s="82" t="s">
+      <c r="F4" s="87"/>
+      <c r="G4" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="83"/>
+      <c r="H4" s="89"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -4177,52 +4174,52 @@
       <c r="K4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="84" t="s">
+      <c r="L4" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="87" t="s">
+      <c r="M4" s="93" t="s">
         <v>133</v>
       </c>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="98" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="100" t="s">
+      <c r="B5" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="100" t="s">
+      <c r="C5" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="67" t="s">
+      <c r="D5" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="80" t="s">
+      <c r="E5" s="86" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="81"/>
-      <c r="G5" s="90" t="s">
+      <c r="F5" s="87"/>
+      <c r="G5" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="91"/>
-      <c r="I5" s="94" t="s">
+      <c r="H5" s="97"/>
+      <c r="I5" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="96" t="s">
+      <c r="J5" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="92" t="s">
+      <c r="K5" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="85"/>
-      <c r="M5" s="88"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="99"/>
-      <c r="B6" s="101"/>
-      <c r="C6" s="101"/>
-      <c r="D6" s="68"/>
+      <c r="L5" s="91"/>
+      <c r="M5" s="94"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="105"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="56"/>
       <c r="E6" s="11" t="s">
         <v>21</v>
       </c>
@@ -4235,140 +4232,140 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="95"/>
-      <c r="J6" s="97"/>
-      <c r="K6" s="93"/>
-      <c r="L6" s="86"/>
-      <c r="M6" s="89"/>
-    </row>
-    <row r="7" spans="1:14" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="102" t="s">
+      <c r="I6" s="101"/>
+      <c r="J6" s="103"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="92"/>
+      <c r="M6" s="95"/>
+    </row>
+    <row r="7" spans="1:14" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="102" t="s">
+      <c r="B7" s="73" t="s">
         <v>141</v>
       </c>
-      <c r="C7" s="102" t="s">
+      <c r="C7" s="73" t="s">
         <v>142</v>
       </c>
-      <c r="D7" s="102" t="s">
+      <c r="D7" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="E7" s="102" t="s">
+      <c r="E7" s="73" t="s">
         <v>151</v>
       </c>
-      <c r="F7" s="102" t="s">
+      <c r="F7" s="73" t="s">
         <v>152</v>
       </c>
-      <c r="G7" s="102" t="s">
+      <c r="G7" s="73" t="s">
         <v>157</v>
       </c>
-      <c r="H7" s="102" t="s">
-        <v>188</v>
-      </c>
-      <c r="I7" s="102"/>
-      <c r="J7" s="102" t="s">
+      <c r="H7" s="73" t="s">
+        <v>187</v>
+      </c>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73" t="s">
         <v>136</v>
       </c>
-      <c r="K7" s="102"/>
-      <c r="L7" s="102" t="s">
+      <c r="K7" s="73"/>
+      <c r="L7" s="73" t="s">
         <v>143</v>
       </c>
       <c r="M7" s="22" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="102"/>
-      <c r="B8" s="102"/>
-      <c r="C8" s="102"/>
-      <c r="D8" s="102"/>
-      <c r="E8" s="102"/>
-      <c r="F8" s="102"/>
-      <c r="G8" s="102"/>
-      <c r="H8" s="102"/>
-      <c r="I8" s="102"/>
-      <c r="J8" s="102"/>
-      <c r="K8" s="102"/>
-      <c r="L8" s="102"/>
+    <row r="8" spans="1:14" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="73"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="73"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="73"/>
       <c r="M8" s="22" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="102"/>
-      <c r="B9" s="102"/>
-      <c r="C9" s="102"/>
-      <c r="D9" s="102"/>
-      <c r="E9" s="102"/>
-      <c r="F9" s="102"/>
-      <c r="G9" s="102"/>
-      <c r="H9" s="102"/>
-      <c r="I9" s="102"/>
-      <c r="J9" s="102"/>
-      <c r="K9" s="102"/>
-      <c r="L9" s="102"/>
+    <row r="9" spans="1:14" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="73"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="73"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
       <c r="M9" s="22" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="102" t="s">
+      <c r="B10" s="73" t="s">
         <v>138</v>
       </c>
-      <c r="C10" s="102" t="s">
+      <c r="C10" s="73" t="s">
         <v>147</v>
       </c>
-      <c r="D10" s="102" t="s">
+      <c r="D10" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="E10" s="102" t="s">
+      <c r="E10" s="73" t="s">
         <v>151</v>
       </c>
-      <c r="F10" s="102" t="s">
+      <c r="F10" s="73" t="s">
         <v>153</v>
       </c>
-      <c r="G10" s="102" t="s">
-        <v>185</v>
-      </c>
-      <c r="H10" s="102" t="s">
-        <v>183</v>
-      </c>
-      <c r="I10" s="102"/>
-      <c r="J10" s="102" t="s">
+      <c r="G10" s="73" t="s">
+        <v>184</v>
+      </c>
+      <c r="H10" s="73" t="s">
+        <v>182</v>
+      </c>
+      <c r="I10" s="73"/>
+      <c r="J10" s="73" t="s">
         <v>139</v>
       </c>
-      <c r="K10" s="102"/>
-      <c r="L10" s="102" t="s">
+      <c r="K10" s="73"/>
+      <c r="L10" s="73" t="s">
         <v>135</v>
       </c>
       <c r="M10" s="22" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="102"/>
-      <c r="C11" s="102"/>
-      <c r="D11" s="102"/>
-      <c r="E11" s="102"/>
-      <c r="F11" s="102"/>
-      <c r="G11" s="102"/>
-      <c r="H11" s="102"/>
-      <c r="I11" s="102"/>
-      <c r="J11" s="102"/>
-      <c r="K11" s="102"/>
-      <c r="L11" s="102"/>
+      <c r="B11" s="73"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="73"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="73"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="73"/>
       <c r="M11" s="22" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="105.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="105.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>31</v>
       </c>
@@ -4388,7 +4385,7 @@
         <v>154</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H12" s="22" t="s">
         <v>159</v>
@@ -4405,7 +4402,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="120.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="120.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
         <v>31</v>
       </c>
@@ -4425,10 +4422,10 @@
         <v>156</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I13" s="22"/>
       <c r="J13" s="22" t="s">
@@ -4444,18 +4441,18 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="L7:L9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="K5:K6"/>
@@ -4472,18 +4469,18 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="L7:L9"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{DE0AC091-170B-4F28-806F-0CE19EF466E0}"/>
@@ -4494,21 +4491,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C279D002CEC08F42B7087C30E58D0266" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e5713f579c7011938dc4987ae8981b8f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3219184d-29ab-4105-b29c-8e343e335d59" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae0a0ff84a3c6712467f60982d6e378d" ns2:_="">
     <xsd:import namespace="3219184d-29ab-4105-b29c-8e343e335d59"/>
@@ -4652,32 +4634,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2038022-656B-4A1B-A485-51A1972238BD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ff57c5a0-3efd-4333-8513-2b909ca014ae"/>
-    <ds:schemaRef ds:uri="0d2457a1-fe8a-4cb2-a5c3-c59e87d2493e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6724C681-8A04-4D66-BB1C-57F7466573C0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AEECCE0-61F9-4782-94C5-382F8EFF459D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4695,6 +4667,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6724C681-8A04-4D66-BB1C-57F7466573C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2038022-656B-4A1B-A485-51A1972238BD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ff57c5a0-3efd-4333-8513-2b909ca014ae"/>
+    <ds:schemaRef ds:uri="0d2457a1-fe8a-4cb2-a5c3-c59e87d2493e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{6ebbfa72-b3b6-4c1f-8b23-058d4f67f013}" enabled="1" method="Privileged" siteId="{bf1ce8b5-5d39-4bc5-ad6e-07b3e4d7d67a}" contentBits="0" removed="0"/>

</xml_diff>

<commit_message>
Actualizacion de las imagenes del flujo de eventos de los event storming mas el tipo de filtrado para agenda y para residente en reservas del enriquesido  (TRABAJO TERMINADO esperamos sea de su agrado y comprención) gracias profesor !
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/Event Storming/ConjuntosResidenciales - Event Storming.xlsx
+++ b/Doo-Doc/Nueva Version Victus/Event Storming/ConjuntosResidenciales - Event Storming.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josez\Documents\Universidad IngeSistemas\Diseño Orientado a Objetos(DOO)\VictusProyect\victus-doc\Doo-Doc\Nueva Version Victus\Event Storming\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\DOO 2024 BD\DOO\victus-doc\Doo-Doc\Nueva Version Victus\Event Storming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A101F4B0-905C-483F-91BD-C56AB6A65D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F016F6-83A1-46EA-B2DF-1A13B637D482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="3" activeTab="5" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
   </bookViews>
   <sheets>
     <sheet name="Flujo de eventos en el tiempo" sheetId="61" r:id="rId1"/>
@@ -1263,85 +1263,190 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1351,111 +1456,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1509,55 +1509,38 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>49333</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>1064</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FE72195-7CEB-38FF-716E-395159B2FE04}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAADC65E-7D29-311B-75D5-D56026F52451}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7917180" cy="6583680"/>
+          <a:ext cx="12241333" cy="7621064"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1864,17 +1847,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EFF4C49-240B-4036-BD62-669D42F23E67}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S31" sqref="S31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.44140625" style="2"/>
+    <col min="1" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1"/>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F18"/>
     </row>
   </sheetData>
@@ -1893,15 +1878,15 @@
       <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" customWidth="1"/>
-    <col min="2" max="2" width="50.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
-    <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>27</v>
       </c>
@@ -1911,7 +1896,7 @@
       <c r="C1" s="37"/>
       <c r="D1" s="38"/>
     </row>
-    <row r="2" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>28</v>
       </c>
@@ -1921,7 +1906,7 @@
       <c r="C2" s="40"/>
       <c r="D2" s="41"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>4</v>
       </c>
@@ -1935,7 +1920,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="73.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
         <v>29</v>
       </c>
@@ -1950,7 +1935,7 @@
         <v>Conjuntos reisdenciales</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>30</v>
       </c>
@@ -1962,7 +1947,7 @@
       </c>
       <c r="D5" s="42"/>
     </row>
-    <row r="6" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>31</v>
       </c>
@@ -1974,7 +1959,7 @@
       </c>
       <c r="D6" s="42"/>
     </row>
-    <row r="7" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
         <v>108</v>
       </c>
@@ -1986,7 +1971,7 @@
       </c>
       <c r="D7" s="42"/>
     </row>
-    <row r="8" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
         <v>109</v>
       </c>
@@ -2024,107 +2009,107 @@
       <selection activeCell="H7" sqref="H7:H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="18.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="36.109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="28.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="36.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.44140625" style="1"/>
+    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="67"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="57"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="68" t="str">
+      <c r="B3" s="64" t="str">
         <f>'Listado Objetos de Dominio'!B4</f>
         <v>Objeto de dominio que representa cada una de las comunidades habitacionales organizadas en un sistema. Abarca la totalidad de los elementos que componen el conjunto, desde las unidades habitacionales individuales (inmuebles) hasta las zonas comunes.</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="68"/>
-      <c r="M3" s="69"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="65"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="53"/>
+      <c r="C4" s="48"/>
       <c r="D4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="54"/>
-      <c r="G4" s="61" t="s">
+      <c r="F4" s="66"/>
+      <c r="G4" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="61"/>
+      <c r="H4" s="51"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -2134,52 +2119,52 @@
       <c r="K4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="64" t="s">
+      <c r="L4" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="65" t="s">
+      <c r="M4" s="55" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="58" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="54" t="s">
+      <c r="E5" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="54"/>
-      <c r="G5" s="59" t="s">
+      <c r="F5" s="66"/>
+      <c r="G5" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="59"/>
-      <c r="I5" s="62" t="s">
+      <c r="H5" s="49"/>
+      <c r="I5" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="63" t="s">
+      <c r="J5" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="60" t="s">
+      <c r="K5" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="64"/>
-      <c r="M5" s="65"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="58"/>
-      <c r="B6" s="53"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="56"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="55"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="47"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="68"/>
       <c r="E6" s="11" t="s">
         <v>21</v>
       </c>
@@ -2192,202 +2177,202 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="62"/>
-      <c r="J6" s="63"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="64"/>
-      <c r="M6" s="65"/>
-    </row>
-    <row r="7" spans="1:14" ht="87.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="50" t="s">
+      <c r="I6" s="52"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="55"/>
+    </row>
+    <row r="7" spans="1:14" ht="87.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="47" t="s">
+      <c r="D7" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="44" t="s">
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="44" t="s">
+      <c r="H7" s="43" t="s">
         <v>158</v>
       </c>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47" t="s">
+      <c r="I7" s="58"/>
+      <c r="J7" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="K7" s="47"/>
-      <c r="L7" s="47" t="s">
+      <c r="K7" s="58"/>
+      <c r="L7" s="58" t="s">
         <v>36</v>
       </c>
       <c r="M7" s="26" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="51"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="48"/>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="62"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="59"/>
+      <c r="L8" s="59"/>
       <c r="M8" s="26" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="51"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="62"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="59"/>
       <c r="M9" s="26" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="51"/>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="43" t="s">
+    <row r="10" spans="1:14" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="62"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="H10" s="43" t="s">
+      <c r="H10" s="69" t="s">
         <v>160</v>
       </c>
-      <c r="I10" s="48"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="48"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="59"/>
       <c r="M10" s="26" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="52"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="49"/>
-      <c r="K11" s="49"/>
-      <c r="L11" s="49"/>
+    <row r="11" spans="1:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="63"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="69"/>
+      <c r="H11" s="69"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="60"/>
       <c r="M11" s="26" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="50" t="s">
+    <row r="12" spans="1:14" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="47" t="s">
+      <c r="C12" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="47" t="s">
+      <c r="D12" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="44" t="s">
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="H12" s="44" t="s">
+      <c r="H12" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="I12" s="47"/>
-      <c r="J12" s="47" t="s">
+      <c r="I12" s="58"/>
+      <c r="J12" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="K12" s="47"/>
-      <c r="L12" s="47" t="s">
+      <c r="K12" s="58"/>
+      <c r="L12" s="58" t="s">
         <v>44</v>
       </c>
       <c r="M12" s="26" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="51"/>
-      <c r="B13" s="48"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="48"/>
+    <row r="13" spans="1:14" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="62"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="59"/>
+      <c r="K13" s="59"/>
+      <c r="L13" s="59"/>
       <c r="M13" s="26" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="51"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="48"/>
+    <row r="14" spans="1:14" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="62"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="59"/>
+      <c r="K14" s="59"/>
+      <c r="L14" s="59"/>
       <c r="M14" s="26" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="52"/>
-      <c r="B15" s="49"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="49"/>
-      <c r="L15" s="49"/>
+    <row r="15" spans="1:14" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="63"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="60"/>
+      <c r="L15" s="60"/>
       <c r="M15" s="26" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36" t="s">
         <v>45</v>
       </c>
@@ -2402,8 +2387,8 @@
       </c>
       <c r="E16" s="35"/>
       <c r="F16" s="35"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
       <c r="I16" s="35"/>
       <c r="J16" s="35" t="s">
         <v>192</v>
@@ -2416,7 +2401,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="99.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>52</v>
       </c>
@@ -2431,10 +2416,10 @@
       </c>
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
-      <c r="G17" s="43" t="s">
+      <c r="G17" s="69" t="s">
         <v>193</v>
       </c>
-      <c r="H17" s="43" t="s">
+      <c r="H17" s="69" t="s">
         <v>160</v>
       </c>
       <c r="I17" s="22"/>
@@ -2449,7 +2434,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>45</v>
       </c>
@@ -2464,8 +2449,8 @@
       </c>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="69"/>
       <c r="I18" s="22"/>
       <c r="J18" s="22" t="s">
         <v>34</v>
@@ -2478,7 +2463,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>31</v>
       </c>
@@ -2493,10 +2478,10 @@
       </c>
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
-      <c r="G19" s="44" t="s">
+      <c r="G19" s="43" t="s">
         <v>194</v>
       </c>
-      <c r="H19" s="44" t="s">
+      <c r="H19" s="43" t="s">
         <v>159</v>
       </c>
       <c r="I19" s="22"/>
@@ -2511,7 +2496,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>31</v>
       </c>
@@ -2526,8 +2511,8 @@
       </c>
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
       <c r="I20" s="22"/>
       <c r="J20" s="22" t="s">
         <v>41</v>
@@ -2540,7 +2525,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>45</v>
       </c>
@@ -2555,8 +2540,8 @@
       </c>
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="46"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="45"/>
       <c r="I21" s="22"/>
       <c r="J21" s="22" t="s">
         <v>36</v>
@@ -2571,6 +2556,37 @@
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="G12:G16"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="G19:G21"/>
+    <mergeCell ref="H19:H21"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="L12:L15"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="I12:I15"/>
+    <mergeCell ref="H12:H16"/>
+    <mergeCell ref="L7:L11"/>
+    <mergeCell ref="K7:K11"/>
+    <mergeCell ref="J7:J11"/>
+    <mergeCell ref="I7:I11"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="C7:C11"/>
     <mergeCell ref="G7:G9"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A5:A6"/>
@@ -2587,37 +2603,6 @@
     <mergeCell ref="B7:B11"/>
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="F7:F11"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="L7:L11"/>
-    <mergeCell ref="K7:K11"/>
-    <mergeCell ref="J7:J11"/>
-    <mergeCell ref="I7:I11"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="L12:L15"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="I12:I15"/>
-    <mergeCell ref="H12:H16"/>
-    <mergeCell ref="G19:G21"/>
-    <mergeCell ref="H19:H21"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="F12:F15"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="G12:G16"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="H17:H18"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
@@ -2639,108 +2624,108 @@
       <selection pane="bottomLeft" activeCell="C13" sqref="C13:C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="1" customWidth="1"/>
     <col min="8" max="8" width="31" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="37.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="37.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.44140625" style="1"/>
+    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="80"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="74"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="81" t="str">
+      <c r="B3" s="75" t="str">
         <f>'Listado Objetos de Dominio'!$B$5</f>
         <v>Objeto de dominio que representa a cada una de las zonas comunes que se encuentran dentro de un conjunto residencial para que los residentes puedan reservar esos espacios y porder usarlos.</v>
       </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="83"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="77"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="85"/>
+      <c r="C4" s="79"/>
       <c r="D4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="86" t="s">
+      <c r="E4" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="87"/>
-      <c r="G4" s="88" t="s">
+      <c r="F4" s="81"/>
+      <c r="G4" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="89"/>
+      <c r="H4" s="83"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -2750,52 +2735,52 @@
       <c r="K4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="90" t="s">
+      <c r="L4" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="93" t="s">
+      <c r="M4" s="87" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="104" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="76" t="s">
+      <c r="B5" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="76" t="s">
+      <c r="C5" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="86" t="s">
+      <c r="E5" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="87"/>
-      <c r="G5" s="96" t="s">
+      <c r="F5" s="81"/>
+      <c r="G5" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="97"/>
-      <c r="I5" s="100" t="s">
+      <c r="H5" s="91"/>
+      <c r="I5" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="102" t="s">
+      <c r="J5" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="98" t="s">
+      <c r="K5" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="91"/>
-      <c r="M5" s="94"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="105"/>
-      <c r="B6" s="77"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="56"/>
+      <c r="L5" s="85"/>
+      <c r="M5" s="88"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="99"/>
+      <c r="B6" s="101"/>
+      <c r="C6" s="101"/>
+      <c r="D6" s="68"/>
       <c r="E6" s="11" t="s">
         <v>21</v>
       </c>
@@ -2808,29 +2793,29 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="101"/>
-      <c r="J6" s="103"/>
-      <c r="K6" s="99"/>
-      <c r="L6" s="92"/>
-      <c r="M6" s="95"/>
-    </row>
-    <row r="7" spans="1:14" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="70" t="s">
+      <c r="I6" s="95"/>
+      <c r="J6" s="97"/>
+      <c r="K6" s="93"/>
+      <c r="L6" s="86"/>
+      <c r="M6" s="89"/>
+    </row>
+    <row r="7" spans="1:14" ht="88.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="105" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="43" t="s">
         <v>161</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="44" t="s">
+      <c r="E7" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="44" t="s">
+      <c r="F7" s="43" t="s">
         <v>62</v>
       </c>
       <c r="G7" s="22" t="s">
@@ -2839,244 +2824,273 @@
       <c r="H7" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44" t="s">
+      <c r="I7" s="43"/>
+      <c r="J7" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="K7" s="44"/>
-      <c r="L7" s="44" t="s">
+      <c r="K7" s="43"/>
+      <c r="L7" s="43" t="s">
         <v>38</v>
       </c>
       <c r="M7" s="24" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="71"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="44" t="s">
+    <row r="8" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="106"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="H8" s="44" t="s">
+      <c r="H8" s="43" t="s">
         <v>163</v>
       </c>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="106" t="s">
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="44"/>
+      <c r="M8" s="70" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="71"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="45"/>
-      <c r="K9" s="45"/>
-      <c r="L9" s="45"/>
-      <c r="M9" s="107"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="72"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="46"/>
-      <c r="K10" s="46"/>
-      <c r="L10" s="46"/>
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="106"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="71"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="107"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="45"/>
       <c r="M10" s="31" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="47" t="s">
+      <c r="C11" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="47" t="s">
+      <c r="D11" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="47" t="s">
+      <c r="E11" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="47" t="s">
+      <c r="F11" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="G11" s="47" t="s">
+      <c r="G11" s="58" t="s">
         <v>164</v>
       </c>
-      <c r="H11" s="47" t="s">
+      <c r="H11" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47" t="s">
+      <c r="I11" s="58"/>
+      <c r="J11" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="K11" s="47"/>
-      <c r="L11" s="47" t="s">
+      <c r="K11" s="58"/>
+      <c r="L11" s="58" t="s">
         <v>37</v>
       </c>
       <c r="M11" s="24" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="49"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="49"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
       <c r="M12" s="32" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="74" t="s">
+    <row r="13" spans="1:14" ht="86.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="103" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="C13" s="47" t="s">
+      <c r="C13" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="D13" s="47" t="s">
+      <c r="D13" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="E13" s="47" t="s">
+      <c r="E13" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="47" t="s">
+      <c r="F13" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="G13" s="44" t="s">
+      <c r="G13" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="H13" s="44" t="s">
+      <c r="H13" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47" t="s">
+      <c r="I13" s="58"/>
+      <c r="J13" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="K13" s="47"/>
-      <c r="L13" s="47" t="s">
+      <c r="K13" s="58"/>
+      <c r="L13" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="M13" s="47" t="s">
+      <c r="M13" s="58" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="75"/>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="49"/>
-      <c r="M14" s="49"/>
-    </row>
-    <row r="15" spans="1:14" ht="120.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="73" t="s">
+    <row r="14" spans="1:14" ht="98.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="104"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="60"/>
+    </row>
+    <row r="15" spans="1:14" ht="120.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="73" t="s">
+      <c r="B15" s="102" t="s">
         <v>176</v>
       </c>
-      <c r="C15" s="73" t="s">
+      <c r="C15" s="102" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="73" t="s">
+      <c r="D15" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="73" t="s">
+      <c r="E15" s="102" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="73" t="s">
+      <c r="F15" s="102" t="s">
         <v>74</v>
       </c>
-      <c r="G15" s="44" t="s">
+      <c r="G15" s="43" t="s">
         <v>165</v>
       </c>
-      <c r="H15" s="44" t="s">
+      <c r="H15" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="I15" s="73"/>
-      <c r="J15" s="73" t="s">
+      <c r="I15" s="102"/>
+      <c r="J15" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="K15" s="73"/>
-      <c r="L15" s="73" t="s">
+      <c r="K15" s="102"/>
+      <c r="L15" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="M15" s="73" t="s">
+      <c r="M15" s="102" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="73"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="73"/>
-      <c r="J16" s="73"/>
-      <c r="K16" s="73"/>
-      <c r="L16" s="73"/>
-      <c r="M16" s="73"/>
+    <row r="16" spans="1:14" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="102"/>
+      <c r="B16" s="102"/>
+      <c r="C16" s="102"/>
+      <c r="D16" s="102"/>
+      <c r="E16" s="102"/>
+      <c r="F16" s="102"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="102"/>
+      <c r="J16" s="102"/>
+      <c r="K16" s="102"/>
+      <c r="L16" s="102"/>
+      <c r="M16" s="102"/>
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="L7:L10"/>
-    <mergeCell ref="K7:K10"/>
-    <mergeCell ref="J7:J10"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I7:I10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="B7:B10"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="B3:M3"/>
@@ -3093,46 +3107,17 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I7:I10"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="L7:L10"/>
+    <mergeCell ref="K7:K10"/>
+    <mergeCell ref="J7:J10"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
@@ -3151,107 +3136,107 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="18.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="31.5546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="43.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="31.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="43.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.44140625" style="1"/>
+    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="67"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="57"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="68" t="str">
+      <c r="B3" s="64" t="str">
         <f>'Listado Objetos de Dominio'!$B$6</f>
         <v xml:space="preserve"> Objeto de dominio que representa el Administrador encargado de hacer la creacion o gestión de las zonas comunes y la gestión de residentes y sus respectivas reservas en caso de ser necesario.</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="68"/>
-      <c r="M3" s="69"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="65"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="53"/>
+      <c r="C4" s="48"/>
       <c r="D4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="54"/>
-      <c r="G4" s="61" t="s">
+      <c r="F4" s="66"/>
+      <c r="G4" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="61"/>
+      <c r="H4" s="51"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -3261,52 +3246,52 @@
       <c r="K4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="64" t="s">
+      <c r="L4" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="65" t="s">
+      <c r="M4" s="55" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="58" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="54" t="s">
+      <c r="E5" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="54"/>
-      <c r="G5" s="59" t="s">
+      <c r="F5" s="66"/>
+      <c r="G5" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="59"/>
-      <c r="I5" s="62" t="s">
+      <c r="H5" s="49"/>
+      <c r="I5" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="63" t="s">
+      <c r="J5" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="60" t="s">
+      <c r="K5" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="64"/>
-      <c r="M5" s="65"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="58"/>
-      <c r="B6" s="53"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="56"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="55"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="47"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="68"/>
       <c r="E6" s="11" t="s">
         <v>21</v>
       </c>
@@ -3319,29 +3304,29 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="62"/>
-      <c r="J6" s="63"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="64"/>
-      <c r="M6" s="65"/>
-    </row>
-    <row r="7" spans="1:14" ht="72" x14ac:dyDescent="0.3">
-      <c r="A7" s="50" t="s">
+      <c r="I6" s="52"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="55"/>
+    </row>
+    <row r="7" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="47" t="s">
+      <c r="D7" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="47" t="s">
+      <c r="E7" s="58" t="s">
         <v>79</v>
       </c>
-      <c r="F7" s="47" t="s">
+      <c r="F7" s="58" t="s">
         <v>80</v>
       </c>
       <c r="G7" s="34" t="s">
@@ -3350,87 +3335,87 @@
       <c r="H7" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47" t="s">
+      <c r="I7" s="58"/>
+      <c r="J7" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="47"/>
-      <c r="L7" s="47" t="s">
+      <c r="K7" s="58"/>
+      <c r="L7" s="58" t="s">
         <v>41</v>
       </c>
       <c r="M7" s="26" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="51"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="44" t="s">
+    <row r="8" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="62"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="H8" s="44" t="s">
+      <c r="H8" s="43" t="s">
         <v>167</v>
       </c>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="48"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="59"/>
+      <c r="L8" s="59"/>
       <c r="M8" s="26" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="51"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="62"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="59"/>
       <c r="M9" s="108" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="51"/>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="48"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="48"/>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="62"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="59"/>
       <c r="M10" s="109"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="52"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="49"/>
-      <c r="K11" s="49"/>
-      <c r="L11" s="49"/>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="63"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="60"/>
       <c r="M11" s="110"/>
     </row>
-    <row r="12" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
         <v>31</v>
       </c>
@@ -3467,63 +3452,63 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="C13" s="47" t="s">
+      <c r="C13" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="D13" s="47" t="s">
+      <c r="D13" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="47" t="s">
+      <c r="E13" s="58" t="s">
         <v>79</v>
       </c>
-      <c r="F13" s="47" t="s">
+      <c r="F13" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="G13" s="73" t="s">
+      <c r="G13" s="102" t="s">
         <v>172</v>
       </c>
-      <c r="H13" s="73" t="s">
+      <c r="H13" s="102" t="s">
         <v>189</v>
       </c>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47" t="s">
+      <c r="I13" s="58"/>
+      <c r="J13" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="K13" s="47"/>
-      <c r="L13" s="47" t="s">
+      <c r="K13" s="58"/>
+      <c r="L13" s="58" t="s">
         <v>104</v>
       </c>
       <c r="M13" s="26" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="73"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="49"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="102"/>
+      <c r="H14" s="102"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
       <c r="M14" s="30" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>31</v>
       </c>
@@ -3560,11 +3545,36 @@
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E16" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L7:L11"/>
+    <mergeCell ref="K7:K11"/>
+    <mergeCell ref="J7:J11"/>
+    <mergeCell ref="I7:I11"/>
+    <mergeCell ref="G8:G11"/>
+    <mergeCell ref="H8:H11"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
     <mergeCell ref="M9:M11"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="A1:N1"/>
@@ -3581,31 +3591,6 @@
     <mergeCell ref="L4:L6"/>
     <mergeCell ref="M4:M6"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L7:L11"/>
-    <mergeCell ref="K7:K11"/>
-    <mergeCell ref="J7:J11"/>
-    <mergeCell ref="I7:I11"/>
-    <mergeCell ref="G8:G11"/>
-    <mergeCell ref="H8:H11"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="F7:F11"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="B7:B11"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
@@ -3622,113 +3607,113 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB345C48-C8D9-4186-9152-4D78F60A6B79}">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="1" customWidth="1"/>
     <col min="8" max="8" width="29" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="37.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="37.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.44140625" style="1"/>
+    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="78" t="str">
+      <c r="B2" s="72" t="str">
         <f>'Listado Objetos de Dominio'!A7</f>
         <v>ZonaInmueble</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="80"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="74"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="81" t="str">
+      <c r="B3" s="75" t="str">
         <f>'Listado Objetos de Dominio'!B7</f>
         <v>Objeto de dominio que representa una Zona de Inmuebles en un conjunto residencial se refiere a una agrupación de unidades habitacionales (como una torre, bloque, o lote) que comparten una ubicación física y características comunes dentro del conjunto.</v>
       </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="83"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="77"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="85"/>
+      <c r="C4" s="79"/>
       <c r="D4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="86" t="s">
+      <c r="E4" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="87"/>
-      <c r="G4" s="88" t="s">
+      <c r="F4" s="81"/>
+      <c r="G4" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="89"/>
+      <c r="H4" s="83"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -3738,52 +3723,52 @@
       <c r="K4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="90" t="s">
+      <c r="L4" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="93" t="s">
+      <c r="M4" s="87" t="s">
         <v>133</v>
       </c>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="104" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="76" t="s">
+      <c r="B5" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="76" t="s">
+      <c r="C5" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="86" t="s">
+      <c r="E5" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="87"/>
-      <c r="G5" s="96" t="s">
+      <c r="F5" s="81"/>
+      <c r="G5" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="97"/>
-      <c r="I5" s="100" t="s">
+      <c r="H5" s="91"/>
+      <c r="I5" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="102" t="s">
+      <c r="J5" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="98" t="s">
+      <c r="K5" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="91"/>
-      <c r="M5" s="94"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="105"/>
-      <c r="B6" s="77"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="56"/>
+      <c r="L5" s="85"/>
+      <c r="M5" s="88"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="99"/>
+      <c r="B6" s="101"/>
+      <c r="C6" s="101"/>
+      <c r="D6" s="68"/>
       <c r="E6" s="11" t="s">
         <v>21</v>
       </c>
@@ -3796,140 +3781,140 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="101"/>
-      <c r="J6" s="103"/>
-      <c r="K6" s="99"/>
-      <c r="L6" s="92"/>
-      <c r="M6" s="95"/>
-    </row>
-    <row r="7" spans="1:14" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="73" t="s">
+      <c r="I6" s="95"/>
+      <c r="J6" s="97"/>
+      <c r="K6" s="93"/>
+      <c r="L6" s="86"/>
+      <c r="M6" s="89"/>
+    </row>
+    <row r="7" spans="1:14" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="102" t="s">
         <v>174</v>
       </c>
-      <c r="C7" s="73" t="s">
+      <c r="C7" s="102" t="s">
         <v>114</v>
       </c>
-      <c r="D7" s="73" t="s">
+      <c r="D7" s="102" t="s">
         <v>108</v>
       </c>
-      <c r="E7" s="73" t="s">
+      <c r="E7" s="102" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="73" t="s">
+      <c r="F7" s="102" t="s">
         <v>115</v>
       </c>
-      <c r="G7" s="73" t="s">
+      <c r="G7" s="102" t="s">
         <v>134</v>
       </c>
-      <c r="H7" s="73" t="s">
+      <c r="H7" s="102" t="s">
         <v>188</v>
       </c>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73" t="s">
+      <c r="I7" s="102"/>
+      <c r="J7" s="102" t="s">
         <v>116</v>
       </c>
-      <c r="K7" s="73"/>
-      <c r="L7" s="73" t="s">
+      <c r="K7" s="102"/>
+      <c r="L7" s="102" t="s">
         <v>117</v>
       </c>
       <c r="M7" s="22" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="73"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="73"/>
-      <c r="H8" s="73"/>
-      <c r="I8" s="73"/>
-      <c r="J8" s="73"/>
-      <c r="K8" s="73"/>
-      <c r="L8" s="73"/>
+    <row r="8" spans="1:14" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="102"/>
+      <c r="B8" s="102"/>
+      <c r="C8" s="102"/>
+      <c r="D8" s="102"/>
+      <c r="E8" s="102"/>
+      <c r="F8" s="102"/>
+      <c r="G8" s="102"/>
+      <c r="H8" s="102"/>
+      <c r="I8" s="102"/>
+      <c r="J8" s="102"/>
+      <c r="K8" s="102"/>
+      <c r="L8" s="102"/>
       <c r="M8" s="22" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="73"/>
-      <c r="B9" s="73"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="73"/>
-      <c r="J9" s="73"/>
-      <c r="K9" s="73"/>
-      <c r="L9" s="73"/>
+    <row r="9" spans="1:14" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="102"/>
+      <c r="B9" s="102"/>
+      <c r="C9" s="102"/>
+      <c r="D9" s="102"/>
+      <c r="E9" s="102"/>
+      <c r="F9" s="102"/>
+      <c r="G9" s="102"/>
+      <c r="H9" s="102"/>
+      <c r="I9" s="102"/>
+      <c r="J9" s="102"/>
+      <c r="K9" s="102"/>
+      <c r="L9" s="102"/>
       <c r="M9" s="22" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="102" t="s">
         <v>121</v>
       </c>
-      <c r="C10" s="73" t="s">
+      <c r="C10" s="102" t="s">
         <v>122</v>
       </c>
-      <c r="D10" s="73" t="s">
+      <c r="D10" s="102" t="s">
         <v>108</v>
       </c>
-      <c r="E10" s="73" t="s">
+      <c r="E10" s="102" t="s">
         <v>63</v>
       </c>
-      <c r="F10" s="73" t="s">
+      <c r="F10" s="102" t="s">
         <v>123</v>
       </c>
-      <c r="G10" s="73" t="s">
+      <c r="G10" s="102" t="s">
         <v>178</v>
       </c>
-      <c r="H10" s="73" t="s">
+      <c r="H10" s="102" t="s">
         <v>183</v>
       </c>
-      <c r="I10" s="73"/>
-      <c r="J10" s="73" t="s">
+      <c r="I10" s="102"/>
+      <c r="J10" s="102" t="s">
         <v>124</v>
       </c>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73" t="s">
+      <c r="K10" s="102"/>
+      <c r="L10" s="102" t="s">
         <v>116</v>
       </c>
       <c r="M10" s="22" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="73"/>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="73"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="73"/>
+      <c r="B11" s="102"/>
+      <c r="C11" s="102"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="102"/>
+      <c r="I11" s="102"/>
+      <c r="J11" s="102"/>
+      <c r="K11" s="102"/>
+      <c r="L11" s="102"/>
       <c r="M11" s="22" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="105.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="105.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>31</v>
       </c>
@@ -3966,7 +3951,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="120.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="120.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>31</v>
       </c>
@@ -4005,6 +3990,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
     <mergeCell ref="L10:L11"/>
     <mergeCell ref="L7:L9"/>
     <mergeCell ref="B10:B11"/>
@@ -4021,30 +4030,6 @@
     <mergeCell ref="K10:K11"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="I7:I9"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="K5:K6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{40DB47AD-DF64-4401-B17F-CC72FC22A8C4}"/>
@@ -4062,109 +4047,109 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="25.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="37.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="37.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.44140625" style="1"/>
+    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="78" t="str">
+      <c r="B2" s="72" t="str">
         <f>'Listado Objetos de Dominio'!A7</f>
         <v>ZonaInmueble</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="80"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="74"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="81" t="str">
+      <c r="B3" s="75" t="str">
         <f>'Listado Objetos de Dominio'!B7</f>
         <v>Objeto de dominio que representa una Zona de Inmuebles en un conjunto residencial se refiere a una agrupación de unidades habitacionales (como una torre, bloque, o lote) que comparten una ubicación física y características comunes dentro del conjunto.</v>
       </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="83"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="77"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="85"/>
+      <c r="C4" s="79"/>
       <c r="D4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="86" t="s">
+      <c r="E4" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="87"/>
-      <c r="G4" s="88" t="s">
+      <c r="F4" s="81"/>
+      <c r="G4" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="89"/>
+      <c r="H4" s="83"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -4174,52 +4159,52 @@
       <c r="K4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="90" t="s">
+      <c r="L4" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="93" t="s">
+      <c r="M4" s="87" t="s">
         <v>133</v>
       </c>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="104" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="76" t="s">
+      <c r="B5" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="76" t="s">
+      <c r="C5" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="86" t="s">
+      <c r="E5" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="87"/>
-      <c r="G5" s="96" t="s">
+      <c r="F5" s="81"/>
+      <c r="G5" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="97"/>
-      <c r="I5" s="100" t="s">
+      <c r="H5" s="91"/>
+      <c r="I5" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="102" t="s">
+      <c r="J5" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="98" t="s">
+      <c r="K5" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="91"/>
-      <c r="M5" s="94"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="105"/>
-      <c r="B6" s="77"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="56"/>
+      <c r="L5" s="85"/>
+      <c r="M5" s="88"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="99"/>
+      <c r="B6" s="101"/>
+      <c r="C6" s="101"/>
+      <c r="D6" s="68"/>
       <c r="E6" s="11" t="s">
         <v>21</v>
       </c>
@@ -4232,140 +4217,140 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="101"/>
-      <c r="J6" s="103"/>
-      <c r="K6" s="99"/>
-      <c r="L6" s="92"/>
-      <c r="M6" s="95"/>
-    </row>
-    <row r="7" spans="1:14" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="73" t="s">
+      <c r="I6" s="95"/>
+      <c r="J6" s="97"/>
+      <c r="K6" s="93"/>
+      <c r="L6" s="86"/>
+      <c r="M6" s="89"/>
+    </row>
+    <row r="7" spans="1:14" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="102" t="s">
         <v>141</v>
       </c>
-      <c r="C7" s="73" t="s">
+      <c r="C7" s="102" t="s">
         <v>142</v>
       </c>
-      <c r="D7" s="73" t="s">
+      <c r="D7" s="102" t="s">
         <v>109</v>
       </c>
-      <c r="E7" s="73" t="s">
+      <c r="E7" s="102" t="s">
         <v>151</v>
       </c>
-      <c r="F7" s="73" t="s">
+      <c r="F7" s="102" t="s">
         <v>152</v>
       </c>
-      <c r="G7" s="73" t="s">
+      <c r="G7" s="102" t="s">
         <v>157</v>
       </c>
-      <c r="H7" s="73" t="s">
+      <c r="H7" s="102" t="s">
         <v>187</v>
       </c>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73" t="s">
+      <c r="I7" s="102"/>
+      <c r="J7" s="102" t="s">
         <v>136</v>
       </c>
-      <c r="K7" s="73"/>
-      <c r="L7" s="73" t="s">
+      <c r="K7" s="102"/>
+      <c r="L7" s="102" t="s">
         <v>143</v>
       </c>
       <c r="M7" s="22" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="73"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="73"/>
-      <c r="H8" s="73"/>
-      <c r="I8" s="73"/>
-      <c r="J8" s="73"/>
-      <c r="K8" s="73"/>
-      <c r="L8" s="73"/>
+    <row r="8" spans="1:14" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="102"/>
+      <c r="B8" s="102"/>
+      <c r="C8" s="102"/>
+      <c r="D8" s="102"/>
+      <c r="E8" s="102"/>
+      <c r="F8" s="102"/>
+      <c r="G8" s="102"/>
+      <c r="H8" s="102"/>
+      <c r="I8" s="102"/>
+      <c r="J8" s="102"/>
+      <c r="K8" s="102"/>
+      <c r="L8" s="102"/>
       <c r="M8" s="22" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="73"/>
-      <c r="B9" s="73"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="73"/>
-      <c r="J9" s="73"/>
-      <c r="K9" s="73"/>
-      <c r="L9" s="73"/>
+    <row r="9" spans="1:14" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="102"/>
+      <c r="B9" s="102"/>
+      <c r="C9" s="102"/>
+      <c r="D9" s="102"/>
+      <c r="E9" s="102"/>
+      <c r="F9" s="102"/>
+      <c r="G9" s="102"/>
+      <c r="H9" s="102"/>
+      <c r="I9" s="102"/>
+      <c r="J9" s="102"/>
+      <c r="K9" s="102"/>
+      <c r="L9" s="102"/>
       <c r="M9" s="22" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="102" t="s">
         <v>138</v>
       </c>
-      <c r="C10" s="73" t="s">
+      <c r="C10" s="102" t="s">
         <v>147</v>
       </c>
-      <c r="D10" s="73" t="s">
+      <c r="D10" s="102" t="s">
         <v>109</v>
       </c>
-      <c r="E10" s="73" t="s">
+      <c r="E10" s="102" t="s">
         <v>151</v>
       </c>
-      <c r="F10" s="73" t="s">
+      <c r="F10" s="102" t="s">
         <v>153</v>
       </c>
-      <c r="G10" s="73" t="s">
+      <c r="G10" s="102" t="s">
         <v>184</v>
       </c>
-      <c r="H10" s="73" t="s">
+      <c r="H10" s="102" t="s">
         <v>182</v>
       </c>
-      <c r="I10" s="73"/>
-      <c r="J10" s="73" t="s">
+      <c r="I10" s="102"/>
+      <c r="J10" s="102" t="s">
         <v>139</v>
       </c>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73" t="s">
+      <c r="K10" s="102"/>
+      <c r="L10" s="102" t="s">
         <v>135</v>
       </c>
       <c r="M10" s="22" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="73"/>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="73"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="73"/>
+      <c r="B11" s="102"/>
+      <c r="C11" s="102"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="102"/>
+      <c r="I11" s="102"/>
+      <c r="J11" s="102"/>
+      <c r="K11" s="102"/>
+      <c r="L11" s="102"/>
       <c r="M11" s="22" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="105.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="105.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>31</v>
       </c>
@@ -4402,7 +4387,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="120.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="120.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>31</v>
       </c>
@@ -4441,18 +4426,18 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="L7:L9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="K5:K6"/>
@@ -4469,18 +4454,18 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="L7:L9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{DE0AC091-170B-4F28-806F-0CE19EF466E0}"/>
@@ -4635,18 +4620,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4668,14 +4653,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6724C681-8A04-4D66-BB1C-57F7466573C0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2038022-656B-4A1B-A485-51A1972238BD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -4692,6 +4669,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6724C681-8A04-4D66-BB1C-57F7466573C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{6ebbfa72-b3b6-4c1f-8b23-058d4f67f013}" enabled="1" method="Privileged" siteId="{bf1ce8b5-5d39-4bc5-ad6e-07b3e4d7d67a}" contentBits="0" removed="0"/>

</xml_diff>